<commit_message>
Teff validation set development
</commit_message>
<xml_diff>
--- a/Prototypes/Teff/Observed.xlsx
+++ b/Prototypes/Teff/Observed.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedHarvestData" sheetId="1" r:id="rId1"/>
     <sheet name="Mekelle2008SW" sheetId="2" r:id="rId2"/>
     <sheet name="Mekelle2008Crop" sheetId="3" r:id="rId3"/>
+    <sheet name="VanDelden" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="134">
   <si>
     <t>SimulationName</t>
   </si>
@@ -392,6 +393,90 @@
   </si>
   <si>
     <t>CoverGreen</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>VanDeldenCvGibePP1</t>
+  </si>
+  <si>
+    <t>VanDeldenCvGibePP2</t>
+  </si>
+  <si>
+    <t>VanDeldenCvGibePP3</t>
+  </si>
+  <si>
+    <t>VanDeldenCvGibePP4</t>
+  </si>
+  <si>
+    <t>VanDeldenCvGibePP5</t>
+  </si>
+  <si>
+    <t>VanDeldenCvGibePP6</t>
+  </si>
+  <si>
+    <t>VanDeldenCvZiqualaPP1</t>
+  </si>
+  <si>
+    <t>VanDeldenCvZiqualaPP2</t>
+  </si>
+  <si>
+    <t>VanDeldenCvZiqualaPP3</t>
+  </si>
+  <si>
+    <t>VanDeldenCvZiqualaPP4</t>
+  </si>
+  <si>
+    <t>VanDeldenCvZiqualaPP5</t>
+  </si>
+  <si>
+    <t>VanDeldenCvZiqualaPP6</t>
+  </si>
+  <si>
+    <t>VanDeldenCvAyanaPP1</t>
+  </si>
+  <si>
+    <t>VanDeldenCvAyanaPP2</t>
+  </si>
+  <si>
+    <t>VanDeldenCvAyanaPP3</t>
+  </si>
+  <si>
+    <t>VanDeldenCvAyanaPP4</t>
+  </si>
+  <si>
+    <t>VanDeldenCvAyanaPP5</t>
+  </si>
+  <si>
+    <t>VanDeldenCvAyanaPP6</t>
+  </si>
+  <si>
+    <t>VanDeldenCv04T19PP1</t>
+  </si>
+  <si>
+    <t>VanDeldenCv04T19PP2</t>
+  </si>
+  <si>
+    <t>VanDeldenCv04T19PP3</t>
+  </si>
+  <si>
+    <t>VanDeldenCv04T19PP4</t>
+  </si>
+  <si>
+    <t>VanDeldenCv04T19PP5</t>
+  </si>
+  <si>
+    <t>VanDeldenCv04T19PP6</t>
+  </si>
+  <si>
+    <t>PanicleInitiationDAS</t>
+  </si>
+  <si>
+    <t>FinalLeafNo</t>
+  </si>
+  <si>
+    <t>InterNodes</t>
   </si>
 </sst>
 </file>
@@ -467,9 +552,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-AU"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -945,23 +1028,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="100025472"/>
-        <c:axId val="100057856"/>
+        <c:axId val="125066624"/>
+        <c:axId val="149262720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="100025472"/>
+        <c:axId val="125066624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100057856"/>
+        <c:crossAx val="149262720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100057856"/>
+        <c:axId val="149262720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -970,7 +1053,242 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100025472"/>
+        <c:crossAx val="125066624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-AU"/>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>VanDelden!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FinalLeafNo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>VanDelden!$B$2:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>16.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>VanDelden!$E$2:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="63510400"/>
+        <c:axId val="63508864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="63510400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="63508864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="63508864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="63510400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -983,7 +1301,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1001,6 +1319,41 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>792480</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
@@ -5490,9 +5843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -5919,4 +6270,498 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+      <c r="E2">
+        <v>7.1</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3">
+        <v>10.5</v>
+      </c>
+      <c r="D3">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="E3">
+        <v>7.2</v>
+      </c>
+      <c r="F3">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="E4">
+        <v>8.5</v>
+      </c>
+      <c r="F4">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>13.5</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>61.5</v>
+      </c>
+      <c r="E5">
+        <v>10.5</v>
+      </c>
+      <c r="F5">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>62</v>
+      </c>
+      <c r="E6">
+        <v>10.6</v>
+      </c>
+      <c r="F6">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7">
+        <v>16.5</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>68.3</v>
+      </c>
+      <c r="E7">
+        <v>10.8</v>
+      </c>
+      <c r="F7">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9">
+        <v>10.5</v>
+      </c>
+      <c r="D9">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E9">
+        <v>8.1</v>
+      </c>
+      <c r="F9">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>44.2</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11">
+        <v>13.5</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>77.2</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+      <c r="F11">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>32</v>
+      </c>
+      <c r="D12">
+        <v>83.8</v>
+      </c>
+      <c r="E12">
+        <v>11.2</v>
+      </c>
+      <c r="F12">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13">
+        <v>16.5</v>
+      </c>
+      <c r="D13">
+        <v>88.3</v>
+      </c>
+      <c r="E13">
+        <v>11.1</v>
+      </c>
+      <c r="F13">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>29.2</v>
+      </c>
+      <c r="E14">
+        <v>6.5</v>
+      </c>
+      <c r="F14">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B15">
+        <v>10.5</v>
+      </c>
+      <c r="D15">
+        <v>30.8</v>
+      </c>
+      <c r="E15">
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>35</v>
+      </c>
+      <c r="E16">
+        <v>7.5</v>
+      </c>
+      <c r="F16">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17">
+        <v>13.5</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>42</v>
+      </c>
+      <c r="E17">
+        <v>7.8</v>
+      </c>
+      <c r="F17">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>44.5</v>
+      </c>
+      <c r="E18">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="F18">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19">
+        <v>16.5</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>44.7</v>
+      </c>
+      <c r="E19">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F19">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>39</v>
+      </c>
+      <c r="E20">
+        <v>8.1</v>
+      </c>
+      <c r="F20">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21">
+        <v>10.5</v>
+      </c>
+      <c r="D21">
+        <v>42.3</v>
+      </c>
+      <c r="E21">
+        <v>8.5</v>
+      </c>
+      <c r="F21">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="D22">
+        <v>44.2</v>
+      </c>
+      <c r="E22">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F22">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23">
+        <v>13.5</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <v>57.3</v>
+      </c>
+      <c r="E23">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="F23">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <v>60.5</v>
+      </c>
+      <c r="E24">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F24">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25">
+        <v>16.5</v>
+      </c>
+      <c r="C25">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>62.3</v>
+      </c>
+      <c r="E25">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="F25">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added met file and progress on mekelle 2008
</commit_message>
<xml_diff>
--- a/Prototypes/Teff/Observed.xlsx
+++ b/Prototypes/Teff/Observed.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedHarvestData" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="ObservedLysimeter2" sheetId="5" r:id="rId5"/>
     <sheet name="ObservedLysimeter4" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -24,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="N64" authorId="0">
+    <comment ref="N64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N67" authorId="0">
+    <comment ref="N67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="144">
   <si>
     <t>SimulationName</t>
   </si>
@@ -506,13 +506,16 @@
   </si>
   <si>
     <t>Lysimeter4</t>
+  </si>
+  <si>
+    <t>LAI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -574,18 +577,40 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
-    <c:title/>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1056,41 +1081,59 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="115873664"/>
-        <c:axId val="115875200"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="206944648"/>
+        <c:axId val="205692408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="115873664"/>
+        <c:axId val="206944648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115875200"/>
+        <c:crossAx val="205692408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="115875200"/>
+        <c:axId val="205692408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="115873664"/>
+        <c:crossAx val="206944648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1102,15 +1145,27 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1292,41 +1347,58 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="116368128"/>
-        <c:axId val="116369664"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="206790744"/>
+        <c:axId val="206791136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116368128"/>
+        <c:axId val="206790744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116369664"/>
+        <c:crossAx val="206791136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116369664"/>
+        <c:axId val="206791136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116368128"/>
+        <c:crossAx val="206790744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1449,7 +1521,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1481,9 +1553,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1515,6 +1588,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1690,7 +1764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S83"/>
   <sheetViews>
     <sheetView topLeftCell="A83" workbookViewId="0">
@@ -1701,7 +1775,7 @@
       <selection pane="bottomRight" activeCell="L57" sqref="L57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
@@ -1711,7 +1785,7 @@
     <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1770,7 +1844,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1807,7 +1881,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1843,7 +1917,7 @@
         <v>142.30000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1879,7 +1953,7 @@
         <v>146.30000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1915,7 +1989,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1951,7 +2025,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1991,7 +2065,7 @@
         <v>85.7</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2031,7 +2105,7 @@
         <v>88.3</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2071,7 +2145,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2111,7 +2185,7 @@
         <v>91.7</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2151,7 +2225,7 @@
         <v>88.7</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2162,7 +2236,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -2173,7 +2247,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -2184,7 +2258,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -2195,7 +2269,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -2206,7 +2280,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -2217,7 +2291,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -2228,7 +2302,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -2239,7 +2313,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
@@ -2250,7 +2324,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -2261,7 +2335,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -2272,7 +2346,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
@@ -2283,7 +2357,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
@@ -2294,7 +2368,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>47</v>
       </c>
@@ -2305,7 +2379,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
@@ -2316,7 +2390,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -2327,7 +2401,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -2338,7 +2412,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
@@ -2349,7 +2423,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -2360,7 +2434,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -2371,7 +2445,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2382,7 +2456,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -2393,7 +2467,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -2404,7 +2478,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>36</v>
       </c>
@@ -2415,7 +2489,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -2426,7 +2500,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
@@ -2437,7 +2511,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -2448,7 +2522,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -2459,7 +2533,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>46</v>
       </c>
@@ -2470,7 +2544,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>48</v>
       </c>
@@ -2481,7 +2555,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -2492,7 +2566,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>52</v>
       </c>
@@ -2503,7 +2577,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -2520,7 +2594,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>87</v>
       </c>
@@ -2537,7 +2611,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>88</v>
       </c>
@@ -2554,7 +2628,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>89</v>
       </c>
@@ -2571,7 +2645,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>90</v>
       </c>
@@ -2588,7 +2662,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>91</v>
       </c>
@@ -2605,7 +2679,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>92</v>
       </c>
@@ -2622,7 +2696,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>93</v>
       </c>
@@ -2639,7 +2713,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>94</v>
       </c>
@@ -2656,7 +2730,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
@@ -2673,7 +2747,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
@@ -2690,7 +2764,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
@@ -2707,7 +2781,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>98</v>
       </c>
@@ -2724,7 +2798,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>99</v>
       </c>
@@ -2741,7 +2815,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>100</v>
       </c>
@@ -2758,7 +2832,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>101</v>
       </c>
@@ -2775,7 +2849,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>53</v>
       </c>
@@ -2792,7 +2866,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>54</v>
       </c>
@@ -2809,7 +2883,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>55</v>
       </c>
@@ -2826,7 +2900,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>56</v>
       </c>
@@ -2843,7 +2917,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>57</v>
       </c>
@@ -2866,7 +2940,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:19">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>58</v>
       </c>
@@ -2883,7 +2957,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="66" spans="1:19">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>59</v>
       </c>
@@ -2900,7 +2974,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="67" spans="1:19">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>60</v>
       </c>
@@ -2923,7 +2997,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:19">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>64</v>
       </c>
@@ -2975,7 +3049,7 @@
         <v>28.85</v>
       </c>
     </row>
-    <row r="69" spans="1:19">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>65</v>
       </c>
@@ -3018,7 +3092,7 @@
         <v>34.43</v>
       </c>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
@@ -3061,7 +3135,7 @@
         <v>36.44</v>
       </c>
     </row>
-    <row r="71" spans="1:19">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
@@ -3104,7 +3178,7 @@
         <v>47.88</v>
       </c>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>68</v>
       </c>
@@ -3147,7 +3221,7 @@
         <v>41.15</v>
       </c>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
@@ -3190,7 +3264,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:19">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>70</v>
       </c>
@@ -3233,7 +3307,7 @@
         <v>50.79</v>
       </c>
     </row>
-    <row r="75" spans="1:19">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>71</v>
       </c>
@@ -3276,7 +3350,7 @@
         <v>45.96</v>
       </c>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>72</v>
       </c>
@@ -3319,7 +3393,7 @@
         <v>46.91</v>
       </c>
     </row>
-    <row r="77" spans="1:19">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>73</v>
       </c>
@@ -3362,7 +3436,7 @@
         <v>46.91</v>
       </c>
     </row>
-    <row r="78" spans="1:19">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>74</v>
       </c>
@@ -3405,7 +3479,7 @@
         <v>37.659999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:19">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>75</v>
       </c>
@@ -3448,7 +3522,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:19">
+    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>76</v>
       </c>
@@ -3491,7 +3565,7 @@
         <v>42.12</v>
       </c>
     </row>
-    <row r="81" spans="1:19">
+    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>77</v>
       </c>
@@ -3534,7 +3608,7 @@
         <v>38.44</v>
       </c>
     </row>
-    <row r="82" spans="1:19">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>78</v>
       </c>
@@ -3577,7 +3651,7 @@
         <v>43.09</v>
       </c>
     </row>
-    <row r="83" spans="1:19">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>79</v>
       </c>
@@ -3630,20 +3704,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.109375" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3657,7 +3731,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="19.2" customHeight="1">
+    <row r="2" spans="1:4" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -3672,7 +3746,7 @@
         <v>100.81699999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
@@ -3687,7 +3761,7 @@
         <v>100.163</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
@@ -3702,7 +3776,7 @@
         <v>103.10599999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>57</v>
       </c>
@@ -3717,7 +3791,7 @@
         <v>97.384200000000007</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>57</v>
       </c>
@@ -3732,7 +3806,7 @@
         <v>96.076300000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
@@ -3747,7 +3821,7 @@
         <v>90.844700000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>57</v>
       </c>
@@ -3762,7 +3836,7 @@
         <v>87.901899999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
@@ -3777,7 +3851,7 @@
         <v>87.084500000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>57</v>
       </c>
@@ -3792,7 +3866,7 @@
         <v>87.084500000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
@@ -3807,7 +3881,7 @@
         <v>87.4114</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
@@ -3822,7 +3896,7 @@
         <v>88.065399999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>57</v>
       </c>
@@ -3837,7 +3911,7 @@
         <v>88.228899999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
@@ -3852,7 +3926,7 @@
         <v>88.228899999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -3867,7 +3941,7 @@
         <v>88.392399999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>57</v>
       </c>
@@ -3882,7 +3956,7 @@
         <v>94.931899999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
@@ -3897,7 +3971,7 @@
         <v>92.97</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
@@ -3912,7 +3986,7 @@
         <v>89.3733</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -3927,7 +4001,7 @@
         <v>89.046300000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>57</v>
       </c>
@@ -3942,7 +4016,7 @@
         <v>95.912800000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -3957,7 +4031,7 @@
         <v>98.692099999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>57</v>
       </c>
@@ -3972,7 +4046,7 @@
         <v>95.095399999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>57</v>
       </c>
@@ -3987,7 +4061,7 @@
         <v>90.027199999999993</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>57</v>
       </c>
@@ -4002,7 +4076,7 @@
         <v>84.632199999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>57</v>
       </c>
@@ -4017,7 +4091,7 @@
         <v>82.997299999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
@@ -4032,7 +4106,7 @@
         <v>79.400499999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>57</v>
       </c>
@@ -4047,7 +4121,7 @@
         <v>75.149900000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>57</v>
       </c>
@@ -4062,7 +4136,7 @@
         <v>73.188000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
@@ -4077,7 +4151,7 @@
         <v>72.697500000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>57</v>
       </c>
@@ -4092,7 +4166,7 @@
         <v>70.899199999999993</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>57</v>
       </c>
@@ -4107,7 +4181,7 @@
         <v>83.978200000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>57</v>
       </c>
@@ -4122,7 +4196,7 @@
         <v>89.209800000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>57</v>
       </c>
@@ -4137,7 +4211,7 @@
         <v>87.5749</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>57</v>
       </c>
@@ -4152,7 +4226,7 @@
         <v>85.776600000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>57</v>
       </c>
@@ -4167,7 +4241,7 @@
         <v>82.670299999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>57</v>
       </c>
@@ -4182,7 +4256,7 @@
         <v>80.871899999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>57</v>
       </c>
@@ -4197,7 +4271,7 @@
         <v>79.727500000000006</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>57</v>
       </c>
@@ -4212,7 +4286,7 @@
         <v>77.111699999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>57</v>
       </c>
@@ -4227,7 +4301,7 @@
         <v>74.005399999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>57</v>
       </c>
@@ -4242,7 +4316,7 @@
         <v>70.245199999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>57</v>
       </c>
@@ -4257,7 +4331,7 @@
         <v>66.975499999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>57</v>
       </c>
@@ -4272,7 +4346,7 @@
         <v>65.013599999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>57</v>
       </c>
@@ -4287,7 +4361,7 @@
         <v>63.0518</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>57</v>
       </c>
@@ -4302,7 +4376,7 @@
         <v>67.302499999999995</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>57</v>
       </c>
@@ -4317,7 +4391,7 @@
         <v>71.389600000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>57</v>
       </c>
@@ -4332,7 +4406,7 @@
         <v>70.245199999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>57</v>
       </c>
@@ -4347,7 +4421,7 @@
         <v>69.264300000000006</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>57</v>
       </c>
@@ -4362,7 +4436,7 @@
         <v>74.005399999999995</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>57</v>
       </c>
@@ -4377,7 +4451,7 @@
         <v>78.419600000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
@@ -4392,7 +4466,7 @@
         <v>73.188000000000002</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>57</v>
       </c>
@@ -4407,7 +4481,7 @@
         <v>74.168899999999994</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>57</v>
       </c>
@@ -4422,7 +4496,7 @@
         <v>69.754800000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -4437,7 +4511,7 @@
         <v>67.138999999999996</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>57</v>
       </c>
@@ -4452,7 +4526,7 @@
         <v>63.0518</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>57</v>
       </c>
@@ -4467,7 +4541,7 @@
         <v>72.370599999999996</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>57</v>
       </c>
@@ -4482,7 +4556,7 @@
         <v>76.9482</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>57</v>
       </c>
@@ -4497,7 +4571,7 @@
         <v>74.332400000000007</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
@@ -4512,7 +4586,7 @@
         <v>72.043599999999998</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
@@ -4527,7 +4601,7 @@
         <v>74.822900000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>57</v>
       </c>
@@ -4542,7 +4616,7 @@
         <v>67.629400000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>57</v>
       </c>
@@ -4557,7 +4631,7 @@
         <v>72.043599999999998</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>57</v>
       </c>
@@ -4572,7 +4646,7 @@
         <v>69.918300000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>57</v>
       </c>
@@ -4587,7 +4661,7 @@
         <v>73.6785</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>57</v>
       </c>
@@ -4602,7 +4676,7 @@
         <v>71.226200000000006</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>57</v>
       </c>
@@ -4617,7 +4691,7 @@
         <v>74.005399999999995</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>57</v>
       </c>
@@ -4632,7 +4706,7 @@
         <v>69.754800000000003</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>57</v>
       </c>
@@ -4647,7 +4721,7 @@
         <v>65.340599999999995</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>57</v>
       </c>
@@ -4662,7 +4736,7 @@
         <v>64.032700000000006</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>57</v>
       </c>
@@ -4677,7 +4751,7 @@
         <v>63.215299999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>57</v>
       </c>
@@ -4692,7 +4766,7 @@
         <v>62.397799999999997</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>57</v>
       </c>
@@ -4707,7 +4781,7 @@
         <v>61.580399999999997</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>57</v>
       </c>
@@ -4722,7 +4796,7 @@
         <v>60.762900000000002</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>57</v>
       </c>
@@ -4737,7 +4811,7 @@
         <v>60.272500000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>57</v>
       </c>
@@ -4752,7 +4826,7 @@
         <v>60.109000000000002</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>53</v>
       </c>
@@ -4767,7 +4841,7 @@
         <v>99.065399999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>53</v>
       </c>
@@ -4782,7 +4856,7 @@
         <v>99.813100000000006</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>53</v>
       </c>
@@ -4797,7 +4871,7 @@
         <v>104.486</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>53</v>
       </c>
@@ -4812,7 +4886,7 @@
         <v>89.532700000000006</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>53</v>
       </c>
@@ -4827,7 +4901,7 @@
         <v>95.140199999999993</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>53</v>
       </c>
@@ -4842,7 +4916,7 @@
         <v>90.093500000000006</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>53</v>
       </c>
@@ -4857,7 +4931,7 @@
         <v>87.289699999999996</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>53</v>
       </c>
@@ -4872,7 +4946,7 @@
         <v>86.355099999999993</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>53</v>
       </c>
@@ -4887,7 +4961,7 @@
         <v>86.728999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>53</v>
       </c>
@@ -4902,7 +4976,7 @@
         <v>86.915899999999993</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>53</v>
       </c>
@@ -4917,7 +4991,7 @@
         <v>86.915899999999993</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>53</v>
       </c>
@@ -4932,7 +5006,7 @@
         <v>87.476600000000005</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>53</v>
       </c>
@@ -4947,7 +5021,7 @@
         <v>87.289699999999996</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>53</v>
       </c>
@@ -4962,7 +5036,7 @@
         <v>90.093500000000006</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>53</v>
       </c>
@@ -4977,7 +5051,7 @@
         <v>90.093500000000006</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>53</v>
       </c>
@@ -4992,7 +5066,7 @@
         <v>94.392499999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>53</v>
       </c>
@@ -5007,7 +5081,7 @@
         <v>96.448599999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>53</v>
       </c>
@@ -5022,7 +5096,7 @@
         <v>94.766400000000004</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>53</v>
       </c>
@@ -5037,7 +5111,7 @@
         <v>88.971999999999994</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>53</v>
       </c>
@@ -5052,7 +5126,7 @@
         <v>96.261700000000005</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>53</v>
       </c>
@@ -5067,7 +5141,7 @@
         <v>97.196299999999994</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>53</v>
       </c>
@@ -5082,7 +5156,7 @@
         <v>92.149500000000003</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>53</v>
       </c>
@@ -5097,7 +5171,7 @@
         <v>87.663600000000002</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>53</v>
       </c>
@@ -5112,7 +5186,7 @@
         <v>87.663600000000002</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -5127,7 +5201,7 @@
         <v>85.981300000000005</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>53</v>
       </c>
@@ -5142,7 +5216,7 @@
         <v>82.616799999999998</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>53</v>
       </c>
@@ -5157,7 +5231,7 @@
         <v>80.747699999999995</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>53</v>
       </c>
@@ -5172,7 +5246,7 @@
         <v>79.252300000000005</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>53</v>
       </c>
@@ -5187,7 +5261,7 @@
         <v>81.121499999999997</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>53</v>
       </c>
@@ -5202,7 +5276,7 @@
         <v>82.803700000000006</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>53</v>
       </c>
@@ -5217,7 +5291,7 @@
         <v>85.981300000000005</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>53</v>
       </c>
@@ -5232,7 +5306,7 @@
         <v>87.663600000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>53</v>
       </c>
@@ -5247,7 +5321,7 @@
         <v>86.168199999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>53</v>
       </c>
@@ -5262,7 +5336,7 @@
         <v>85.046700000000001</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>53</v>
       </c>
@@ -5277,7 +5351,7 @@
         <v>81.869200000000006</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>53</v>
       </c>
@@ -5292,7 +5366,7 @@
         <v>82.616799999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>53</v>
       </c>
@@ -5307,7 +5381,7 @@
         <v>83.177599999999998</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>53</v>
       </c>
@@ -5322,7 +5396,7 @@
         <v>80.373800000000003</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>53</v>
       </c>
@@ -5337,7 +5411,7 @@
         <v>77.196299999999994</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>53</v>
       </c>
@@ -5352,7 +5426,7 @@
         <v>77.009299999999996</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>53</v>
       </c>
@@ -5367,7 +5441,7 @@
         <v>76.635499999999993</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>53</v>
       </c>
@@ -5382,7 +5456,7 @@
         <v>73.084100000000007</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>53</v>
       </c>
@@ -5397,7 +5471,7 @@
         <v>70.2804</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>53</v>
       </c>
@@ -5412,7 +5486,7 @@
         <v>71.215000000000003</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>53</v>
       </c>
@@ -5427,7 +5501,7 @@
         <v>72.523399999999995</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>53</v>
       </c>
@@ -5442,7 +5516,7 @@
         <v>72.897199999999998</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>53</v>
       </c>
@@ -5457,7 +5531,7 @@
         <v>73.457899999999995</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>53</v>
       </c>
@@ -5472,7 +5546,7 @@
         <v>71.215000000000003</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>53</v>
       </c>
@@ -5487,7 +5561,7 @@
         <v>69.345799999999997</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>53</v>
       </c>
@@ -5502,7 +5576,7 @@
         <v>65.981300000000005</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>53</v>
       </c>
@@ -5517,7 +5591,7 @@
         <v>65.046700000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>53</v>
       </c>
@@ -5532,7 +5606,7 @@
         <v>63.551400000000001</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>53</v>
       </c>
@@ -5547,7 +5621,7 @@
         <v>62.616799999999998</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>53</v>
       </c>
@@ -5562,7 +5636,7 @@
         <v>60.373800000000003</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>53</v>
       </c>
@@ -5577,7 +5651,7 @@
         <v>58.5047</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>53</v>
       </c>
@@ -5592,7 +5666,7 @@
         <v>58.130800000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>53</v>
       </c>
@@ -5607,7 +5681,7 @@
         <v>57.570099999999996</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>53</v>
       </c>
@@ -5622,7 +5696,7 @@
         <v>56.074800000000003</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>53</v>
       </c>
@@ -5637,7 +5711,7 @@
         <v>54.018700000000003</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>53</v>
       </c>
@@ -5652,7 +5726,7 @@
         <v>53.831800000000001</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>53</v>
       </c>
@@ -5667,7 +5741,7 @@
         <v>52.710299999999997</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>53</v>
       </c>
@@ -5682,7 +5756,7 @@
         <v>51.775700000000001</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>53</v>
       </c>
@@ -5697,7 +5771,7 @@
         <v>51.588799999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>53</v>
       </c>
@@ -5712,7 +5786,7 @@
         <v>50.467300000000002</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>53</v>
       </c>
@@ -5727,7 +5801,7 @@
         <v>49.532699999999998</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>53</v>
       </c>
@@ -5742,7 +5816,7 @@
         <v>49.158900000000003</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>53</v>
       </c>
@@ -5757,7 +5831,7 @@
         <v>49.158900000000003</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>53</v>
       </c>
@@ -5772,7 +5846,7 @@
         <v>48.037399999999998</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>53</v>
       </c>
@@ -5787,7 +5861,7 @@
         <v>47.663600000000002</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>53</v>
       </c>
@@ -5802,7 +5876,7 @@
         <v>45.607500000000002</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>53</v>
       </c>
@@ -5817,7 +5891,7 @@
         <v>46.168199999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>53</v>
       </c>
@@ -5832,7 +5906,7 @@
         <v>46.168199999999999</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>53</v>
       </c>
@@ -5847,7 +5921,7 @@
         <v>46.542099999999998</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>53</v>
       </c>
@@ -5869,18 +5943,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5897,10 +5973,16 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1">
+      <c r="H1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
@@ -5919,7 +6001,7 @@
         <v>99.289299999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
@@ -5927,18 +6009,18 @@
         <v>40.525700000000001</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C24" si="0">DATE(2008,8,2)+B3</f>
+        <f t="shared" ref="C3:C26" si="0">DATE(2008,8,2)+B3</f>
         <v>39702.525699999998</v>
       </c>
       <c r="D3">
         <v>2.2404999999999999</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E13" si="1">D3*1000/10</f>
+        <f t="shared" ref="E3:E14" si="1">D3*1000/10</f>
         <v>224.05</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -5957,7 +6039,7 @@
         <v>358.42600000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -5976,7 +6058,7 @@
         <v>413.959</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
@@ -5995,7 +6077,7 @@
         <v>400.255</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -6014,287 +6096,364 @@
         <v>373.08800000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B8">
+        <f>B7+C8-C7+1</f>
+        <v>96</v>
+      </c>
+      <c r="C8" s="1">
+        <v>39757</v>
+      </c>
+      <c r="E8">
+        <v>393</v>
+      </c>
+      <c r="F8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9">
         <v>30.723299999999998</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>39692.723299999998</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>1.2620899999999999</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <f t="shared" si="1"/>
         <v>126.20899999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
         <v>40.367600000000003</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>39702.367599999998</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>2.2597700000000001</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <f t="shared" si="1"/>
         <v>225.977</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
         <v>50.486199999999997</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>39712.486199999999</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>3.77657</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <f t="shared" si="1"/>
         <v>377.65700000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12">
         <v>60.130400000000002</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>39722.130400000002</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>5.4857899999999997</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <f t="shared" si="1"/>
         <v>548.57899999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
         <v>70.248999999999995</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>39732.249000000003</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>7.07951</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <f t="shared" si="1"/>
         <v>707.95100000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14">
         <v>80.525700000000001</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>39742.525699999998</v>
       </c>
-      <c r="D13">
+      <c r="D14">
         <v>7.6154999999999999</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f t="shared" si="1"/>
         <v>761.55</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15">
+        <f>B14+C15-C14+1</f>
+        <v>96</v>
+      </c>
+      <c r="C15" s="1">
+        <v>39757</v>
+      </c>
+      <c r="E15">
+        <v>762</v>
+      </c>
+      <c r="F15">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16">
         <v>30.393999999999998</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C16" s="1">
         <f t="shared" si="0"/>
         <v>39692.394</v>
       </c>
-      <c r="F14">
+      <c r="G16">
         <v>0.32997599999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15">
+      <c r="H16">
+        <f t="shared" ref="H16:H21" si="2">LN(1-G16)/-0.65</f>
+        <v>0.61606422514331682</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17">
         <v>40.268099999999997</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C17" s="1">
         <f t="shared" si="0"/>
         <v>39702.268100000001</v>
       </c>
-      <c r="F15">
+      <c r="G17">
         <v>0.61774600000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16">
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>1.4794922613414281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18">
         <v>50.530500000000004</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C18" s="1">
         <f t="shared" si="0"/>
         <v>39712.530500000001</v>
       </c>
-      <c r="F16">
+      <c r="G18">
         <v>0.69256600000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17">
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>1.8146074598755551</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
         <v>60.320399999999999</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C19" s="1">
         <f t="shared" si="0"/>
         <v>39722.320399999997</v>
       </c>
-      <c r="F17">
+      <c r="G19">
         <v>0.57362099999999994</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18">
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>1.3114256259603951</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20">
         <v>70.379000000000005</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C20" s="1">
         <f t="shared" si="0"/>
         <v>39732.379000000001</v>
       </c>
-      <c r="F18">
+      <c r="G20">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19">
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
         <v>30.383299999999998</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C21" s="1">
         <f t="shared" si="0"/>
         <v>39692.383300000001</v>
       </c>
-      <c r="F19">
+      <c r="G21">
         <v>0.37985599999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20">
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>0.73508241514801897</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22">
         <v>40.103000000000002</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C22" s="1">
         <f t="shared" si="0"/>
         <v>39702.103000000003</v>
       </c>
-      <c r="F20">
+      <c r="G22">
         <v>0.58896900000000008</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21">
+      <c r="H22">
+        <f t="shared" ref="H22:H26" si="3">LN(1-G22)/-0.65</f>
+        <v>1.367825602368508</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23">
         <v>50.537500000000001</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C23" s="1">
         <f t="shared" si="0"/>
         <v>39712.537499999999</v>
       </c>
-      <c r="F21">
+      <c r="G23">
         <v>0.65995199999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22">
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>1.6594899921012336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24">
         <v>60.292099999999998</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C24" s="1">
         <f t="shared" si="0"/>
         <v>39722.292099999999</v>
       </c>
-      <c r="F22">
+      <c r="G24">
         <v>0.70599500000000004</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23">
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>1.883320776900536</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25">
         <v>70.395899999999997</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C25" s="1">
         <f t="shared" si="0"/>
         <v>39732.395900000003</v>
       </c>
-      <c r="F23">
+      <c r="G25">
         <v>0.72134299999999996</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24">
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>1.9658056064037499</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26">
         <v>80.339399999999998</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C26" s="1">
         <f t="shared" si="0"/>
         <v>39742.339399999997</v>
       </c>
-      <c r="F24">
+      <c r="G26">
         <v>0.68489199999999995</v>
       </c>
-    </row>
-    <row r="1048576" spans="1:1">
-      <c r="A1048576" s="2"/>
+      <c r="H26">
+        <f t="shared" si="3"/>
+        <v>1.7766766796549629</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6302,19 +6461,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6334,7 +6493,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -6354,7 +6513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -6371,7 +6530,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -6388,7 +6547,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -6408,7 +6567,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -6428,7 +6587,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -6448,7 +6607,7 @@
         <v>6.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -6468,7 +6627,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -6485,7 +6644,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -6502,7 +6661,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -6522,7 +6681,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -6542,7 +6701,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -6559,7 +6718,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>119</v>
       </c>
@@ -6579,7 +6738,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -6596,7 +6755,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>121</v>
       </c>
@@ -6613,7 +6772,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>122</v>
       </c>
@@ -6633,7 +6792,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>123</v>
       </c>
@@ -6653,7 +6812,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>124</v>
       </c>
@@ -6673,7 +6832,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>125</v>
       </c>
@@ -6693,7 +6852,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -6710,7 +6869,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -6727,7 +6886,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>128</v>
       </c>
@@ -6747,7 +6906,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>129</v>
       </c>
@@ -6767,7 +6926,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>130</v>
       </c>
@@ -6794,19 +6953,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6838,7 +6997,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -6871,7 +7030,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -6904,7 +7063,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -6937,7 +7096,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>141</v>
       </c>
@@ -6970,7 +7129,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -7003,7 +7162,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>141</v>
       </c>
@@ -7036,7 +7195,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>141</v>
       </c>
@@ -7069,7 +7228,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -7102,7 +7261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -7135,7 +7294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>141</v>
       </c>
@@ -7168,7 +7327,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -7201,7 +7360,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -7234,7 +7393,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>141</v>
       </c>
@@ -7267,7 +7426,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>141</v>
       </c>
@@ -7300,7 +7459,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>141</v>
       </c>
@@ -7333,7 +7492,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>141</v>
       </c>
@@ -7372,19 +7531,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7416,7 +7575,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -7449,7 +7608,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -7482,7 +7641,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -7515,7 +7674,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -7548,7 +7707,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>142</v>
       </c>
@@ -7581,7 +7740,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -7614,7 +7773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>142</v>
       </c>
@@ -7647,7 +7806,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -7680,7 +7839,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>142</v>
       </c>
@@ -7713,7 +7872,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -7746,7 +7905,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>142</v>
       </c>
@@ -7779,7 +7938,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>142</v>
       </c>
@@ -7812,7 +7971,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -7845,13 +8004,13 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Grain DM and N growth
</commit_message>
<xml_diff>
--- a/Prototypes/Teff/Observed.xlsx
+++ b/Prototypes/Teff/Observed.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedHarvestData" sheetId="1" r:id="rId1"/>
     <sheet name="Mekelle2008SW" sheetId="2" r:id="rId2"/>
-    <sheet name="Mekelle2008Crop" sheetId="3" r:id="rId3"/>
-    <sheet name="VanDelden" sheetId="4" r:id="rId4"/>
-    <sheet name="ObservedLysimeter2" sheetId="5" r:id="rId5"/>
-    <sheet name="ObservedLysimeter4" sheetId="6" r:id="rId6"/>
+    <sheet name="CWP2010" sheetId="7" r:id="rId3"/>
+    <sheet name="Mekelle2008Crop" sheetId="3" r:id="rId4"/>
+    <sheet name="VanDelden" sheetId="4" r:id="rId5"/>
+    <sheet name="ObservedLysimeter2" sheetId="5" r:id="rId6"/>
+    <sheet name="ObservedLysimeter4" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -603,7 +604,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -616,467 +645,111 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Mekelle2008SW!$D$1</c:f>
+              <c:f>ObservedHarvestData!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SW30cm</c:v>
+                  <c:v>BiomassN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Mekelle2008SW!$B$2:$B$74</c:f>
+              <c:f>ObservedHarvestData!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>4.2721099999999996</c:v>
+                  <c:v>219.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4868499999999996</c:v>
+                  <c:v>317</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.57456</c:v>
+                  <c:v>500.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.5076200000000002</c:v>
+                  <c:v>689.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.8560300000000005</c:v>
+                  <c:v>517.70000000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.6550600000000006</c:v>
+                  <c:v>571.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.5944</c:v>
+                  <c:v>790.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.6736</c:v>
+                  <c:v>939.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.7006</c:v>
+                  <c:v>965.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.782500000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15.0542</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16.405899999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>17.351900000000001</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>18.5685</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>19.664300000000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>20.605799999999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>21.678799999999999</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>22.7591</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>23.720500000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>24.8079</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>25.880800000000001</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>26.545100000000001</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>27.478899999999999</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>28.5563</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>29.4941</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>30.5657</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>31.507200000000001</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>32.722299999999997</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>33.799300000000002</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>34.774700000000003</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>35.732500000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>36.809899999999999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>37.481499999999997</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>38.420400000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>39.497500000000002</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>40.440800000000003</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>41.515999999999998</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>42.5901</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>43.5276</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>44.601300000000002</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>45.677999999999997</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>46.619500000000002</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>47.439900000000002</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>48.395000000000003</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>49.3384</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>50.2821</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>51.373899999999999</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>52.6</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>53.399099999999997</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>55.563400000000001</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>56.634599999999999</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>57.439500000000002</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>58.376199999999997</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>59.343200000000003</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>60.569699999999997</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>61.2395</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>62.315399999999997</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>63.673000000000002</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>64.602800000000002</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>65.423500000000004</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>66.499799999999993</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>67.589399999999998</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>68.529799999999994</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>69.211699999999993</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>70.283199999999994</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>71.354399999999998</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>72.162199999999999</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>73.511700000000005</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>74.4559</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>75.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>76.479200000000006</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>77.559200000000004</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>78.639899999999997</c:v>
+                  <c:v>803.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Mekelle2008SW!$D$2:$D$74</c:f>
+              <c:f>ObservedHarvestData!$H$2:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="73"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>100.81699999999999</c:v>
+                  <c:v>20.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100.163</c:v>
+                  <c:v>41.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>103.10599999999999</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>97.384200000000007</c:v>
+                  <c:v>81.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.076300000000003</c:v>
+                  <c:v>61.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>90.844700000000003</c:v>
+                  <c:v>70.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87.901899999999998</c:v>
+                  <c:v>119.49</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>87.084500000000006</c:v>
+                  <c:v>167.19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>87.084500000000006</c:v>
+                  <c:v>205.89</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>87.4114</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>88.065399999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>88.228899999999996</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>88.228899999999996</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>88.392399999999995</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>94.931899999999999</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>92.97</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>89.3733</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>89.046300000000002</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>95.912800000000004</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>98.692099999999996</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>95.095399999999998</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>90.027199999999993</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>84.632199999999997</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>82.997299999999996</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>79.400499999999994</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>75.149900000000002</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>73.188000000000002</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>72.697500000000005</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>70.899199999999993</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>83.978200000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>89.209800000000001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>87.5749</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>85.776600000000002</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>82.670299999999997</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>80.871899999999997</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>79.727500000000006</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>77.111699999999999</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>74.005399999999995</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>70.245199999999997</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>66.975499999999997</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>65.013599999999997</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>63.0518</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>67.302499999999995</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>71.389600000000002</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>70.245199999999997</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>69.264300000000006</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>74.005399999999995</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>78.419600000000003</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>73.188000000000002</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>74.168899999999994</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>69.754800000000003</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>67.138999999999996</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>63.0518</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>72.370599999999996</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>76.9482</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>74.332400000000007</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>72.043599999999998</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>74.822900000000004</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>67.629400000000004</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>72.043599999999998</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>69.918300000000002</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>73.6785</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>71.226200000000006</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>74.005399999999995</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>69.754800000000003</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>65.340599999999995</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>64.032700000000006</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>63.215299999999999</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>62.397799999999997</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>61.580399999999997</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>60.762900000000002</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>60.272500000000001</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>60.109000000000002</c:v>
+                  <c:v>131.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1091,53 +764,173 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="206944648"/>
-        <c:axId val="205692408"/>
+        <c:axId val="527644352"/>
+        <c:axId val="527643960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="206944648"/>
+        <c:axId val="527644352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="205692408"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="527643960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="205692408"/>
+        <c:axId val="527643960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="40"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206944648"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="527644352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1158,6 +951,564 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Mekelle2008SW!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SW30cm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Mekelle2008SW!$B$2:$B$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="73"/>
+                <c:pt idx="0">
+                  <c:v>4.2721099999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4868499999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.57456</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5076200000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.8560300000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6550600000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.5944</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.6736</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.7006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14.782500000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15.0542</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.405899999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.351900000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>18.5685</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.664300000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20.605799999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21.678799999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22.7591</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23.720500000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>24.8079</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25.880800000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>26.545100000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27.478899999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>28.5563</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29.4941</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>30.5657</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31.507200000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>32.722299999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>33.799300000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34.774700000000003</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35.732500000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>36.809899999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37.481499999999997</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>38.420400000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>39.497500000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>40.440800000000003</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41.515999999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>42.5901</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>43.5276</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>44.601300000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45.677999999999997</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>46.619500000000002</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>47.439900000000002</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>48.395000000000003</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>49.3384</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>50.2821</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>51.373899999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>52.6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>53.399099999999997</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>55.563400000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>56.634599999999999</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>57.439500000000002</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>58.376199999999997</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>59.343200000000003</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>60.569699999999997</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>61.2395</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>62.315399999999997</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>63.673000000000002</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>64.602800000000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>65.423500000000004</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>66.499799999999993</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>67.589399999999998</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>68.529799999999994</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>69.211699999999993</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>70.283199999999994</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>71.354399999999998</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>72.162199999999999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>73.511700000000005</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>74.4559</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>75.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>76.479200000000006</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>77.559200000000004</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>78.639899999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Mekelle2008SW!$D$2:$D$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="73"/>
+                <c:pt idx="0">
+                  <c:v>100.81699999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.163</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>103.10599999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.384200000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.076300000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90.844700000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87.901899999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>87.084500000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>87.084500000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>87.4114</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>88.065399999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>88.228899999999996</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88.228899999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>88.392399999999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94.931899999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>92.97</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>89.3733</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>89.046300000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95.912800000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>98.692099999999996</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>95.095399999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>90.027199999999993</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>84.632199999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>82.997299999999996</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>79.400499999999994</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>75.149900000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>73.188000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>72.697500000000005</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>70.899199999999993</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>83.978200000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>89.209800000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>87.5749</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>85.776600000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>82.670299999999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>80.871899999999997</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>79.727500000000006</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>77.111699999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>74.005399999999995</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>70.245199999999997</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>66.975499999999997</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>65.013599999999997</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>63.0518</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>67.302499999999995</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>71.389600000000002</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>70.245199999999997</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>69.264300000000006</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>74.005399999999995</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>78.419600000000003</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>73.188000000000002</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>74.168899999999994</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>69.754800000000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>67.138999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>63.0518</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>72.370599999999996</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>76.9482</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>74.332400000000007</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>72.043599999999998</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>74.822900000000004</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>67.629400000000004</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>72.043599999999998</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>69.918300000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>73.6785</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>71.226200000000006</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>74.005399999999995</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>69.754800000000003</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65.340599999999995</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>64.032700000000006</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>63.215299999999999</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>62.397799999999997</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>61.580399999999997</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>60.762900000000002</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>60.272500000000001</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>60.109000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="188077120"/>
+        <c:axId val="188077512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="188077120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188077512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="188077512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="40"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="188077120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1357,11 +1708,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="206790744"/>
-        <c:axId val="206791136"/>
+        <c:axId val="188079864"/>
+        <c:axId val="188083000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="206790744"/>
+        <c:axId val="188079864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1371,12 +1722,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206791136"/>
+        <c:crossAx val="188083000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206791136"/>
+        <c:axId val="188083000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1387,13 +1738,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="206790744"/>
+        <c:crossAx val="188079864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1408,7 +1760,598 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1443,7 +2386,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1767,12 +2710,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S83"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <pane xSplit="5400" ySplit="576" topLeftCell="J50" activePane="bottomRight"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <pane xSplit="5400" ySplit="576" topLeftCell="B1" activePane="bottomRight"/>
       <selection activeCell="A83" sqref="A83"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
-      <selection pane="bottomRight" activeCell="L57" sqref="L57"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3699,7 +4642,8 @@
     <sortCondition ref="A2:A67"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5944,9 +6888,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -6460,7 +7416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -6952,7 +7908,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
@@ -7530,7 +8486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added CWP cover data
</commit_message>
<xml_diff>
--- a/Prototypes/Teff/Observed.xlsx
+++ b/Prototypes/Teff/Observed.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedHarvestData" sheetId="1" r:id="rId1"/>
-    <sheet name="Mekelle2008SW" sheetId="2" r:id="rId2"/>
-    <sheet name="CWP2010" sheetId="7" r:id="rId3"/>
+    <sheet name="CWP2010" sheetId="8" r:id="rId2"/>
+    <sheet name="Mekelle2008SW" sheetId="2" r:id="rId3"/>
     <sheet name="Mekelle2008Crop" sheetId="3" r:id="rId4"/>
     <sheet name="VanDelden" sheetId="4" r:id="rId5"/>
     <sheet name="ObservedLysimeter2" sheetId="5" r:id="rId6"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="144">
   <si>
     <t>SimulationName</t>
   </si>
@@ -606,353 +606,6 @@
     <c:title>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ObservedHarvestData!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>BiomassN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>ObservedHarvestData!$D$2:$D$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>219.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>317</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>500.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>689.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>517.70000000000005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>571.9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>790.4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>939.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>965.2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>803.8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>ObservedHarvestData!$H$2:$H$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>20.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41.4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>62</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>81.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>61.6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>70.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>119.49</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>167.19</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>205.89</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>131.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="527644352"/>
-        <c:axId val="527643960"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="527644352"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="527643960"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="527643960"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="527644352"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1440,11 +1093,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188077120"/>
-        <c:axId val="188077512"/>
+        <c:axId val="190348568"/>
+        <c:axId val="190348952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188077120"/>
+        <c:axId val="190348568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,12 +1107,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188077512"/>
+        <c:crossAx val="190348952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188077512"/>
+        <c:axId val="190348952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -1471,7 +1124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188077120"/>
+        <c:crossAx val="190348568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1493,7 +1146,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1508,7 +1161,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1708,11 +1360,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="188079864"/>
-        <c:axId val="188083000"/>
+        <c:axId val="190021408"/>
+        <c:axId val="190021792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="188079864"/>
+        <c:axId val="190021408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,12 +1374,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188083000"/>
+        <c:crossAx val="190021792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="188083000"/>
+        <c:axId val="190021792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1738,14 +1390,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="188079864"/>
+        <c:crossAx val="190021408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1760,598 +1411,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2386,7 +1446,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2710,12 +1770,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <pane xSplit="5400" ySplit="576" topLeftCell="B1" activePane="bottomRight"/>
+    <sheetView topLeftCell="A83" workbookViewId="0">
+      <pane xSplit="5400" ySplit="576" topLeftCell="B1" activePane="bottomLeft"/>
       <selection activeCell="A83" sqref="A83"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:A15"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4642,12 +3702,885 @@
     <sortCondition ref="A2:A67"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1">
+        <f>DATE(2010,12,1)+B2</f>
+        <v>40531</v>
+      </c>
+      <c r="G2">
+        <v>0.100411</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ref="H2:H28" si="0">LN(1-G2)/-0.65</f>
+        <v>0.16279582558226338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C33" si="1">DATE(2010,12,1)+B3</f>
+        <v>40543</v>
+      </c>
+      <c r="G3">
+        <v>0.49978700000000004</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>1.0657250327264367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="1"/>
+        <v>40554</v>
+      </c>
+      <c r="G4">
+        <v>0.80300700000000003</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2.4993647444159759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>51</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="1"/>
+        <v>40564</v>
+      </c>
+      <c r="G5">
+        <v>0.90274399999999999</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>3.5852440026594521</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="1"/>
+        <v>40574</v>
+      </c>
+      <c r="G6">
+        <v>0.95303899999999997</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>4.7052889368770998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>71</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="1"/>
+        <v>40584</v>
+      </c>
+      <c r="G7">
+        <v>0.95683200000000002</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>4.8348550753181421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>81</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="1"/>
+        <v>40594</v>
+      </c>
+      <c r="G8">
+        <v>0.60590699999999997</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1.4325667029665659</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1">
+        <f>DATE(2010,12,1)+B9</f>
+        <v>40531</v>
+      </c>
+      <c r="G9">
+        <v>0.10197300000000001</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.16546945279506198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="1"/>
+        <v>40543</v>
+      </c>
+      <c r="G10">
+        <v>0.50231199999999998</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1.0735106220284432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="1"/>
+        <v>40554</v>
+      </c>
+      <c r="G11">
+        <v>0.80115599999999998</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>2.4849764327404271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>51</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="1"/>
+        <v>40564</v>
+      </c>
+      <c r="G12">
+        <v>0.89999499999999999</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>3.5423616834523135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>61</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="1"/>
+        <v>40574</v>
+      </c>
+      <c r="G13">
+        <v>0.90608599999999995</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>3.6390397063073214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>71</v>
+      </c>
+      <c r="C14" s="1">
+        <f t="shared" si="1"/>
+        <v>40584</v>
+      </c>
+      <c r="G14">
+        <v>0.90347100000000002</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>3.5967873809984794</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <v>81</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" si="1"/>
+        <v>40594</v>
+      </c>
+      <c r="G15">
+        <v>0.60232399999999997</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1.4186425778225658</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>18</v>
+      </c>
+      <c r="C16" s="1">
+        <f>DATE(2010,12,1)+B16</f>
+        <v>40531</v>
+      </c>
+      <c r="G16">
+        <v>0.100436</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.16283858074367979</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="1"/>
+        <v>40543</v>
+      </c>
+      <c r="G17">
+        <v>0.45323200000000002</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.92881645870226348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>41</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="1"/>
+        <v>40554</v>
+      </c>
+      <c r="G18">
+        <v>0.70411600000000008</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>1.8735196820917912</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>51</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="1"/>
+        <v>40564</v>
+      </c>
+      <c r="G19">
+        <v>0.80382699999999996</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>2.5057820861531415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>61</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="1"/>
+        <v>40574</v>
+      </c>
+      <c r="G20">
+        <v>0.85994799999999993</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>3.0242176873291071</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21">
+        <v>71</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="1"/>
+        <v>40584</v>
+      </c>
+      <c r="G21">
+        <v>0.80850300000000008</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>2.5428971327392174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>81</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="1"/>
+        <v>40594</v>
+      </c>
+      <c r="G22">
+        <v>0.55935299999999999</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1.2607864270523148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>18</v>
+      </c>
+      <c r="C23" s="1">
+        <f>DATE(2010,12,1)+B23</f>
+        <v>40531</v>
+      </c>
+      <c r="G23">
+        <v>0.10513400000000001</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>0.17089429628758651</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="1"/>
+        <v>40543</v>
+      </c>
+      <c r="G24">
+        <v>0.40342300000000003</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>0.79468762990480768</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>41</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="1"/>
+        <v>40554</v>
+      </c>
+      <c r="G25">
+        <v>0.60146699999999997</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>1.4153307286783807</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>51</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="1"/>
+        <v>40564</v>
+      </c>
+      <c r="G26">
+        <v>0.704156</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>1.8737276778656335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>61</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="1"/>
+        <v>40574</v>
+      </c>
+      <c r="G27">
+        <v>0.70171099999999997</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>1.861065328876798</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>71</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="1"/>
+        <v>40584</v>
+      </c>
+      <c r="G28">
+        <v>0.400978</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>0.78839531332513868</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>81</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="1"/>
+        <v>40594</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="1"/>
+        <v>40543</v>
+      </c>
+      <c r="D30">
+        <v>1.4170700000000001</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ref="E30:E45" si="2">D30*1000/10</f>
+        <v>141.70700000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31">
+        <v>50</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="1"/>
+        <v>40563</v>
+      </c>
+      <c r="D31">
+        <v>3.6139299999999999</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>361.39299999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="1"/>
+        <v>40573</v>
+      </c>
+      <c r="D32">
+        <v>3.7926299999999999</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>379.26300000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33">
+        <v>70</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" si="1"/>
+        <v>40583</v>
+      </c>
+      <c r="D33">
+        <v>4.6190899999999999</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>461.90899999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" ref="C34:C37" si="3">DATE(2010,12,1)+B34</f>
+        <v>40543</v>
+      </c>
+      <c r="D34">
+        <v>1.44414</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>144.41399999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35">
+        <v>50</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" si="3"/>
+        <v>40563</v>
+      </c>
+      <c r="D35">
+        <v>3.59673</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>359.673</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36">
+        <v>60</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" si="3"/>
+        <v>40573</v>
+      </c>
+      <c r="D36">
+        <v>3.7874699999999999</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>378.74699999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>70</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" si="3"/>
+        <v>40583</v>
+      </c>
+      <c r="D37">
+        <v>4.5776599999999998</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>457.76599999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38">
+        <v>30</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" ref="C38:C45" si="4">DATE(2010,12,1)+B38</f>
+        <v>40543</v>
+      </c>
+      <c r="D38">
+        <v>1.3342000000000001</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>133.42000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39">
+        <v>50</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" si="4"/>
+        <v>40563</v>
+      </c>
+      <c r="D39">
+        <v>3.1973600000000002</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>319.73599999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40">
+        <v>60</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" si="4"/>
+        <v>40573</v>
+      </c>
+      <c r="D40">
+        <v>3.1684000000000001</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>316.84000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41">
+        <v>70</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" si="4"/>
+        <v>40583</v>
+      </c>
+      <c r="D41">
+        <v>4.0340999999999996</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>403.40999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" si="4"/>
+        <v>40543</v>
+      </c>
+      <c r="D42">
+        <v>1.2139200000000001</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>121.39200000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B43">
+        <v>50</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" si="4"/>
+        <v>40563</v>
+      </c>
+      <c r="D43">
+        <v>2.4078400000000002</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>240.78400000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44">
+        <v>60</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" si="4"/>
+        <v>40573</v>
+      </c>
+      <c r="D44">
+        <v>2.8452000000000002</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>284.52000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45">
+        <v>70</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" si="4"/>
+        <v>40583</v>
+      </c>
+      <c r="D45">
+        <v>3.2087599999999998</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>320.87599999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D148"/>
   <sheetViews>
@@ -6886,24 +6819,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added ETc data to datasets
</commit_message>
<xml_diff>
--- a/Prototypes/Teff/Observed.xlsx
+++ b/Prototypes/Teff/Observed.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedHarvestData" sheetId="1" r:id="rId1"/>
     <sheet name="CWP2010" sheetId="8" r:id="rId2"/>
-    <sheet name="Mekelle2008SW" sheetId="2" r:id="rId3"/>
-    <sheet name="Mekelle2008Crop" sheetId="3" r:id="rId4"/>
-    <sheet name="VanDelden" sheetId="4" r:id="rId5"/>
-    <sheet name="ObservedLysimeter2" sheetId="5" r:id="rId6"/>
-    <sheet name="ObservedLysimeter4" sheetId="6" r:id="rId7"/>
+    <sheet name="MekelleET" sheetId="9" r:id="rId3"/>
+    <sheet name="Mekelle2008SW" sheetId="2" r:id="rId4"/>
+    <sheet name="Mekelle2008Crop" sheetId="3" r:id="rId5"/>
+    <sheet name="VanDelden" sheetId="4" r:id="rId6"/>
+    <sheet name="ObservedLysimeter2" sheetId="5" r:id="rId7"/>
+    <sheet name="ObservedLysimeter4" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="145">
   <si>
     <t>SimulationName</t>
   </si>
@@ -510,6 +511,9 @@
   </si>
   <si>
     <t>LAI</t>
+  </si>
+  <si>
+    <t>Zadok</t>
   </si>
 </sst>
 </file>
@@ -565,13 +569,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,11 +1098,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190348568"/>
-        <c:axId val="190348952"/>
+        <c:axId val="202768960"/>
+        <c:axId val="202769344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="190348568"/>
+        <c:axId val="202768960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1107,12 +1112,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190348952"/>
+        <c:crossAx val="202769344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190348952"/>
+        <c:axId val="202769344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -1124,7 +1129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190348568"/>
+        <c:crossAx val="202768960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1360,11 +1365,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="190021408"/>
-        <c:axId val="190021792"/>
+        <c:axId val="202690008"/>
+        <c:axId val="202694488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="190021408"/>
+        <c:axId val="202690008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,12 +1379,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190021792"/>
+        <c:crossAx val="202694488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="190021792"/>
+        <c:axId val="202694488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1390,7 +1395,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="190021408"/>
+        <c:crossAx val="202690008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3710,9 +3715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E45"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4582,11 +4585,402 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <f>DATE(2008,8,2)+B2</f>
+        <v>39669</v>
+      </c>
+      <c r="D2">
+        <v>2.508</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C14" si="0">DATE(2008,8,2)+B3</f>
+        <v>39676</v>
+      </c>
+      <c r="D3">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>39683</v>
+      </c>
+      <c r="D4">
+        <v>2.82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>39690</v>
+      </c>
+      <c r="D5">
+        <v>3.2280000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>39697</v>
+      </c>
+      <c r="D6">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>39704</v>
+      </c>
+      <c r="D7">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>39711</v>
+      </c>
+      <c r="D8">
+        <v>4.056</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9">
+        <v>56</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>39718</v>
+      </c>
+      <c r="D9">
+        <v>4.6680000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>63</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>39725</v>
+      </c>
+      <c r="D10">
+        <v>4.8120000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
+        <v>70</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>39732</v>
+      </c>
+      <c r="D11">
+        <v>3.972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12">
+        <v>77</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>39739</v>
+      </c>
+      <c r="D12">
+        <v>1.944</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <v>84</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>39746</v>
+      </c>
+      <c r="D13">
+        <v>0.76800000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1">
+        <f>DATE(2009,7,31)+B14</f>
+        <v>40032</v>
+      </c>
+      <c r="D14">
+        <v>2.6549700000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <f t="shared" ref="C15:C25" si="1">DATE(2009,7,31)+B15</f>
+        <v>40039</v>
+      </c>
+      <c r="D15">
+        <v>3.08772</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1">
+        <f t="shared" si="1"/>
+        <v>40046</v>
+      </c>
+      <c r="D16">
+        <v>3.3801199999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1">
+        <f t="shared" si="1"/>
+        <v>40053</v>
+      </c>
+      <c r="D17">
+        <v>3.8713500000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1">
+        <f t="shared" si="1"/>
+        <v>40060</v>
+      </c>
+      <c r="D18">
+        <v>3.8830399999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1">
+        <f t="shared" si="1"/>
+        <v>40067</v>
+      </c>
+      <c r="D19">
+        <v>4.7836299999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20">
+        <v>49</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" si="1"/>
+        <v>40074</v>
+      </c>
+      <c r="D20">
+        <v>5.2865500000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="1"/>
+        <v>40081</v>
+      </c>
+      <c r="D21">
+        <v>5.4853800000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="1"/>
+        <v>40088</v>
+      </c>
+      <c r="D22">
+        <v>4.9239800000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23">
+        <v>70</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="1"/>
+        <v>40095</v>
+      </c>
+      <c r="D23">
+        <v>4.3508800000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24">
+        <v>77</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="1"/>
+        <v>40102</v>
+      </c>
+      <c r="D24">
+        <v>2.5731000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25">
+        <v>84</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="1"/>
+        <v>40109</v>
+      </c>
+      <c r="D25">
+        <v>0.76023399999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6819,12 +7213,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6833,7 +7227,7 @@
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6858,8 +7252,11 @@
       <c r="H1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
@@ -6878,7 +7275,7 @@
         <v>99.289299999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>53</v>
       </c>
@@ -6897,7 +7294,7 @@
         <v>224.05</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -6916,7 +7313,7 @@
         <v>358.42600000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -6935,7 +7332,7 @@
         <v>413.959</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
@@ -6954,7 +7351,7 @@
         <v>400.255</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -6973,7 +7370,7 @@
         <v>373.08800000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>53</v>
       </c>
@@ -6991,7 +7388,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
@@ -7010,7 +7407,7 @@
         <v>126.20899999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>57</v>
       </c>
@@ -7029,7 +7426,7 @@
         <v>225.977</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
@@ -7048,7 +7445,7 @@
         <v>377.65700000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>57</v>
       </c>
@@ -7067,7 +7464,7 @@
         <v>548.57899999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>57</v>
       </c>
@@ -7086,7 +7483,7 @@
         <v>707.95100000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
@@ -7105,7 +7502,7 @@
         <v>761.55</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -7123,7 +7520,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>53</v>
       </c>
@@ -7142,7 +7539,7 @@
         <v>0.61606422514331682</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>53</v>
       </c>
@@ -7161,7 +7558,7 @@
         <v>1.4794922613414281</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>53</v>
       </c>
@@ -7180,7 +7577,7 @@
         <v>1.8146074598755551</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -7199,7 +7596,7 @@
         <v>1.3114256259603951</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>53</v>
       </c>
@@ -7218,7 +7615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>57</v>
       </c>
@@ -7237,7 +7634,7 @@
         <v>0.73508241514801897</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>57</v>
       </c>
@@ -7256,7 +7653,7 @@
         <v>1.367825602368508</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>57</v>
       </c>
@@ -7275,7 +7672,7 @@
         <v>1.6594899921012336</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>57</v>
       </c>
@@ -7294,7 +7691,7 @@
         <v>1.883320776900536</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>57</v>
       </c>
@@ -7313,7 +7710,7 @@
         <v>1.9658056064037499</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>57</v>
       </c>
@@ -7330,6 +7727,94 @@
       <c r="H26">
         <f t="shared" si="3"/>
         <v>1.7766766796549629</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="4">
+        <v>39668</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="1">
+        <v>39708</v>
+      </c>
+      <c r="I28">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="1">
+        <v>39749</v>
+      </c>
+      <c r="I29">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1">
+        <v>39757</v>
+      </c>
+      <c r="I30">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="1">
+        <v>39938</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1">
+        <v>40069</v>
+      </c>
+      <c r="I32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="1">
+        <v>40053</v>
+      </c>
+      <c r="I33">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="1">
+        <v>40132</v>
+      </c>
+      <c r="I34">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -7337,7 +7822,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -7829,7 +8314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
@@ -8407,7 +8892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>

</xml_diff>

<commit_message>
Trying to get canopy working
</commit_message>
<xml_diff>
--- a/Prototypes/Teff/Observed.xlsx
+++ b/Prototypes/Teff/Observed.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedHarvestData" sheetId="1" r:id="rId1"/>
-    <sheet name="CWP2010" sheetId="8" r:id="rId2"/>
-    <sheet name="MekelleET" sheetId="9" r:id="rId3"/>
-    <sheet name="Mekelle2008SW" sheetId="2" r:id="rId4"/>
-    <sheet name="Mekelle2008Crop" sheetId="3" r:id="rId5"/>
-    <sheet name="VanDelden" sheetId="4" r:id="rId6"/>
-    <sheet name="ObservedLysimeter2" sheetId="5" r:id="rId7"/>
-    <sheet name="ObservedLysimeter4" sheetId="6" r:id="rId8"/>
+    <sheet name="Phenology" sheetId="10" r:id="rId2"/>
+    <sheet name="Canopy" sheetId="12" r:id="rId3"/>
+    <sheet name="CWP2010" sheetId="8" r:id="rId4"/>
+    <sheet name="MekelleET" sheetId="9" r:id="rId5"/>
+    <sheet name="Mekelle2008SW" sheetId="2" r:id="rId6"/>
+    <sheet name="Mekelle2008Crop" sheetId="3" r:id="rId7"/>
+    <sheet name="VanDelden" sheetId="4" r:id="rId8"/>
+    <sheet name="ObservedLysimeter2" sheetId="5" r:id="rId9"/>
+    <sheet name="ObservedLysimeter4" sheetId="6" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -26,7 +28,31 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="N64" authorId="0" shapeId="0">
+    <comment ref="O27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Added 8 days because this is half the length of the flowering period</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -46,11 +72,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Start of flowering</t>
+Start of flowering so add 8 days which is the duration of flowering suggested in the paper</t>
         </r>
       </text>
     </comment>
-    <comment ref="N67" authorId="0" shapeId="0">
+    <comment ref="O67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +96,89 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Start of flowering</t>
+Start of flowering so add 8 days which is the duration of flowering suggested in the paper</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B7" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Added 8 days because this is half the length of the flowering period</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Added 8 days because this is half the length of the flowering period</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Added 8 days because this is half the length of the flowering period</t>
         </r>
       </text>
     </comment>
@@ -79,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="149">
   <si>
     <t>SimulationName</t>
   </si>
@@ -514,13 +622,25 @@
   </si>
   <si>
     <t>Zadok</t>
+  </si>
+  <si>
+    <t>GrainNConc</t>
+  </si>
+  <si>
+    <t>Clock.Today</t>
+  </si>
+  <si>
+    <t>Teff.Leaf.CoverGreen</t>
+  </si>
+  <si>
+    <t>Teff.Leaf.LAI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -548,6 +668,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -569,7 +702,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -578,6 +711,9 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1098,11 +1234,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201005096"/>
-        <c:axId val="201005488"/>
+        <c:axId val="438485656"/>
+        <c:axId val="438486048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201005096"/>
+        <c:axId val="438485656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1112,12 +1248,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201005488"/>
+        <c:crossAx val="438486048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201005488"/>
+        <c:axId val="438486048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -1129,7 +1265,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201005096"/>
+        <c:crossAx val="438485656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1364,11 +1500,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199746808"/>
-        <c:axId val="199747200"/>
+        <c:axId val="438487616"/>
+        <c:axId val="438488008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="199746808"/>
+        <c:axId val="438487616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1378,12 +1514,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199747200"/>
+        <c:crossAx val="438488008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199747200"/>
+        <c:axId val="438488008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1394,7 +1530,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199746808"/>
+        <c:crossAx val="438487616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1772,27 +1908,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S83"/>
+  <dimension ref="A1:T83"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
-      <pane xSplit="5400" ySplit="576" topLeftCell="B1" activePane="bottomLeft"/>
-      <selection activeCell="A83" sqref="A83"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12:A15"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1815,43 +1948,46 @@
         <v>62</v>
       </c>
       <c r="H1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>85</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>81</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>82</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1869,26 +2005,30 @@
         <v>143.69999999999999</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>1.5</v>
       </c>
       <c r="H2">
-        <v>20.2</v>
+        <f>G2/(E2)</f>
+        <v>1.9736842105263157E-2</v>
       </c>
       <c r="I2">
-        <f>H2-G2</f>
-        <v>5.1999999999999993</v>
-      </c>
-      <c r="M2">
+        <v>2.02</v>
+      </c>
+      <c r="J2">
+        <f>I2-G2</f>
+        <v>0.52</v>
+      </c>
+      <c r="N2">
         <v>68.7</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>76.7</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1905,26 +2045,30 @@
         <v>201.2</v>
       </c>
       <c r="G3">
-        <v>31.7</v>
+        <v>3.17</v>
       </c>
       <c r="H3">
-        <v>41.4</v>
+        <f t="shared" ref="H3:H11" si="0">G3/(E3)</f>
+        <v>2.7374784110535406E-2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I11" si="0">H3-G3</f>
-        <v>9.6999999999999993</v>
-      </c>
-      <c r="M3">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J11" si="1">I3-G3</f>
+        <v>0.96999999999999975</v>
+      </c>
+      <c r="N3">
         <v>72</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>81.3</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>142.30000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1941,26 +2085,30 @@
         <v>304.5</v>
       </c>
       <c r="G4">
-        <v>48.3</v>
+        <v>4.83</v>
       </c>
       <c r="H4">
-        <v>62</v>
+        <f t="shared" si="0"/>
+        <v>2.4605196128374935E-2</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>13.700000000000003</v>
-      </c>
-      <c r="M4">
+        <v>6.2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>1.37</v>
+      </c>
+      <c r="N4">
         <v>76</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>85</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>146.30000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1977,26 +2125,30 @@
         <v>435.5</v>
       </c>
       <c r="G5">
-        <v>62.5</v>
+        <v>6.25</v>
       </c>
       <c r="H5">
-        <v>81.2</v>
+        <f t="shared" si="0"/>
+        <v>2.461599054745963E-2</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
-        <v>18.700000000000003</v>
-      </c>
-      <c r="M5">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>1.8699999999999992</v>
+      </c>
+      <c r="N5">
         <v>80.7</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>90</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2013,26 +2165,30 @@
         <v>305.89999999999998</v>
       </c>
       <c r="G6">
-        <v>46.6</v>
+        <v>4.66</v>
       </c>
       <c r="H6">
-        <v>61.6</v>
+        <f t="shared" si="0"/>
+        <v>2.2001888574126535E-2</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="M6">
+        <v>6.16</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="N6">
         <v>74</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>83.3</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2049,30 +2205,34 @@
         <v>360.8</v>
       </c>
       <c r="G7">
-        <v>24.7</v>
+        <v>2.4700000000000002</v>
       </c>
       <c r="H7">
-        <v>70.5</v>
+        <f t="shared" si="0"/>
+        <v>1.1700615821885363E-2</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
-        <v>45.8</v>
-      </c>
-      <c r="K7">
-        <f>E7/10/L7</f>
+        <v>7.05</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>4.58</v>
+      </c>
+      <c r="L7">
+        <f>E7/10/M7</f>
         <v>84440</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>56.3</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>85.7</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2089,30 +2249,34 @@
         <v>507.3</v>
       </c>
       <c r="G8">
-        <v>63.69</v>
+        <v>6.3689999999999998</v>
       </c>
       <c r="H8">
-        <v>119.49</v>
+        <f t="shared" si="0"/>
+        <v>2.2497350759448954E-2</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
-        <v>55.8</v>
-      </c>
-      <c r="K8">
-        <f>E8/10/L8</f>
+        <v>11.949</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>5.58</v>
+      </c>
+      <c r="L8">
+        <f>E8/10/M8</f>
         <v>104851.85185185185</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>2.7E-4</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>58</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>88.3</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2129,30 +2293,34 @@
         <v>601.20000000000005</v>
       </c>
       <c r="G9">
-        <v>87.19</v>
+        <v>8.7189999999999994</v>
       </c>
       <c r="H9">
-        <v>167.19</v>
+        <f t="shared" si="0"/>
+        <v>2.579585798816568E-2</v>
       </c>
       <c r="I9">
-        <f t="shared" si="0"/>
-        <v>80</v>
-      </c>
-      <c r="K9">
-        <f>E9/10/L9</f>
+        <v>16.719000000000001</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000018</v>
+      </c>
+      <c r="L9">
+        <f>E9/10/M9</f>
         <v>109032.25806451612</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>3.1E-4</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>60.7</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2169,30 +2337,34 @@
         <v>620.79999999999995</v>
       </c>
       <c r="G10">
-        <v>92.29</v>
+        <v>9.2289999999999992</v>
       </c>
       <c r="H10">
-        <v>205.89</v>
+        <f t="shared" si="0"/>
+        <v>2.6797328687572588E-2</v>
       </c>
       <c r="I10">
-        <f t="shared" si="0"/>
-        <v>113.59999999999998</v>
-      </c>
-      <c r="K10">
-        <f>E10/10/L10</f>
+        <v>20.588999999999999</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>11.36</v>
+      </c>
+      <c r="L10">
+        <f>E10/10/M10</f>
         <v>98400</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>3.5E-4</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>61.7</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>91.7</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2209,30 +2381,34 @@
         <v>512</v>
       </c>
       <c r="G11">
-        <v>70.599999999999994</v>
+        <v>7.06</v>
       </c>
       <c r="H11">
-        <v>131.5</v>
+        <f t="shared" si="0"/>
+        <v>2.4194653872515418E-2</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
-        <v>60.900000000000006</v>
-      </c>
-      <c r="K11">
-        <f>E11/10/L11</f>
+        <v>13.15</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>6.0900000000000007</v>
+      </c>
+      <c r="L11">
+        <f>E11/10/M11</f>
         <v>104214.28571428572</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>2.7999999999999998E-4</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>57.3</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>88.7</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2243,7 +2419,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -2254,7 +2430,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -2265,7 +2441,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -2276,7 +2452,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -2287,7 +2463,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -2298,7 +2474,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -2309,7 +2485,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -2320,7 +2496,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
@@ -2331,7 +2507,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -2342,7 +2518,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -2353,7 +2529,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
@@ -2364,7 +2540,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
@@ -2375,7 +2551,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>47</v>
       </c>
@@ -2386,7 +2562,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
@@ -2397,7 +2573,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -2407,8 +2583,14 @@
       <c r="E27">
         <v>285</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="O27">
+        <v>56</v>
+      </c>
+      <c r="P27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -2419,7 +2601,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
@@ -2430,7 +2612,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -2441,7 +2623,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -2452,7 +2634,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2669,7 +2851,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>91</v>
       </c>
@@ -2686,7 +2868,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>92</v>
       </c>
@@ -2703,7 +2885,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>93</v>
       </c>
@@ -2720,7 +2902,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>94</v>
       </c>
@@ -2737,7 +2919,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
@@ -2754,7 +2936,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
@@ -2771,7 +2953,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
@@ -2788,7 +2970,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>98</v>
       </c>
@@ -2805,7 +2987,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>99</v>
       </c>
@@ -2822,7 +3004,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>100</v>
       </c>
@@ -2839,7 +3021,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>101</v>
       </c>
@@ -2856,7 +3038,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>53</v>
       </c>
@@ -2873,7 +3055,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>54</v>
       </c>
@@ -2890,7 +3072,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>55</v>
       </c>
@@ -2907,7 +3089,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>56</v>
       </c>
@@ -2924,7 +3106,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>57</v>
       </c>
@@ -2940,14 +3122,15 @@
       <c r="F64">
         <v>567</v>
       </c>
-      <c r="N64">
-        <v>46</v>
-      </c>
       <c r="O64">
+        <f>46+8</f>
+        <v>54</v>
+      </c>
+      <c r="P64">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>58</v>
       </c>
@@ -2964,7 +3147,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>59</v>
       </c>
@@ -2981,7 +3164,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>60</v>
       </c>
@@ -2997,14 +3180,15 @@
       <c r="F67">
         <v>440</v>
       </c>
-      <c r="N67">
-        <v>44</v>
-      </c>
       <c r="O67">
+        <f>44+8</f>
+        <v>52</v>
+      </c>
+      <c r="P67">
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>64</v>
       </c>
@@ -3023,40 +3207,40 @@
       <c r="G68">
         <v>18.3</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>31.5</v>
       </c>
-      <c r="I68">
-        <f t="shared" ref="I68:I83" si="1">H68-G68</f>
+      <c r="J68">
+        <f t="shared" ref="J68:J83" si="2">I68-G68</f>
         <v>13.2</v>
       </c>
-      <c r="K68">
-        <f>E12/10/L68</f>
+      <c r="L68">
+        <f>E12/10/M68</f>
         <v>100831.60083160082</v>
       </c>
-      <c r="L68">
+      <c r="M68">
         <v>2.8860000000000002E-4</v>
       </c>
-      <c r="M68">
+      <c r="N68">
         <v>48</v>
       </c>
-      <c r="O68">
+      <c r="P68">
         <v>84.8</v>
       </c>
-      <c r="P68">
+      <c r="Q68">
         <v>5.47</v>
       </c>
-      <c r="Q68">
+      <c r="R68">
         <v>7.73</v>
       </c>
-      <c r="R68">
+      <c r="S68">
         <v>95.75</v>
       </c>
-      <c r="S68">
+      <c r="T68">
         <v>28.85</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>65</v>
       </c>
@@ -3076,30 +3260,31 @@
       <c r="G69" s="3">
         <v>24.53</v>
       </c>
-      <c r="H69" s="3">
+      <c r="H69" s="3"/>
+      <c r="I69" s="3">
         <v>46.24</v>
       </c>
-      <c r="I69">
-        <f t="shared" si="1"/>
+      <c r="J69">
+        <f t="shared" si="2"/>
         <v>21.71</v>
       </c>
-      <c r="M69" s="3">
+      <c r="N69" s="3">
         <v>49.33</v>
       </c>
-      <c r="P69" s="3">
+      <c r="Q69" s="3">
         <v>4.67</v>
       </c>
-      <c r="Q69" s="3">
+      <c r="R69" s="3">
         <v>11.33</v>
       </c>
-      <c r="R69" s="3">
+      <c r="S69" s="3">
         <v>112.58</v>
       </c>
-      <c r="S69" s="3">
+      <c r="T69" s="3">
         <v>34.43</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
@@ -3119,30 +3304,31 @@
       <c r="G70" s="3">
         <v>25.24</v>
       </c>
-      <c r="H70" s="3">
+      <c r="H70" s="3"/>
+      <c r="I70" s="3">
         <v>45.94</v>
       </c>
-      <c r="I70">
-        <f t="shared" si="1"/>
+      <c r="J70">
+        <f t="shared" si="2"/>
         <v>20.7</v>
       </c>
-      <c r="M70" s="3">
+      <c r="N70" s="3">
         <v>53.33</v>
       </c>
-      <c r="P70" s="3">
+      <c r="Q70" s="3">
         <v>5.33</v>
       </c>
-      <c r="Q70" s="3">
+      <c r="R70" s="3">
         <v>17.329999999999998</v>
       </c>
-      <c r="R70" s="3">
+      <c r="S70" s="3">
         <v>113.25</v>
       </c>
-      <c r="S70" s="3">
+      <c r="T70" s="3">
         <v>36.44</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
@@ -3162,30 +3348,31 @@
       <c r="G71" s="3">
         <v>27.2</v>
       </c>
-      <c r="H71" s="3">
+      <c r="H71" s="3"/>
+      <c r="I71" s="3">
         <v>57.84</v>
       </c>
-      <c r="I71">
-        <f t="shared" si="1"/>
+      <c r="J71">
+        <f t="shared" si="2"/>
         <v>30.640000000000004</v>
       </c>
-      <c r="M71" s="3">
+      <c r="N71" s="3">
         <v>52</v>
       </c>
-      <c r="P71" s="3">
+      <c r="Q71" s="3">
         <v>7.33</v>
       </c>
-      <c r="Q71" s="3">
+      <c r="R71" s="3">
         <v>17</v>
       </c>
-      <c r="R71" s="3">
+      <c r="S71" s="3">
         <v>112.22</v>
       </c>
-      <c r="S71" s="3">
+      <c r="T71" s="3">
         <v>47.88</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>68</v>
       </c>
@@ -3205,30 +3392,31 @@
       <c r="G72" s="3">
         <v>27.61</v>
       </c>
-      <c r="H72" s="3">
+      <c r="H72" s="3"/>
+      <c r="I72" s="3">
         <v>50.72</v>
       </c>
-      <c r="I72">
-        <f t="shared" si="1"/>
+      <c r="J72">
+        <f t="shared" si="2"/>
         <v>23.11</v>
       </c>
-      <c r="M72" s="3">
+      <c r="N72" s="3">
         <v>52.67</v>
       </c>
-      <c r="P72" s="3">
+      <c r="Q72" s="3">
         <v>6</v>
       </c>
-      <c r="Q72" s="3">
+      <c r="R72" s="3">
         <v>15</v>
       </c>
-      <c r="R72" s="3">
+      <c r="S72" s="3">
         <v>113.41</v>
       </c>
-      <c r="S72" s="3">
+      <c r="T72" s="3">
         <v>41.15</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
@@ -3248,30 +3436,31 @@
       <c r="G73" s="3">
         <v>29.28</v>
       </c>
-      <c r="H73" s="3">
+      <c r="H73" s="3"/>
+      <c r="I73" s="3">
         <v>59.99</v>
       </c>
-      <c r="I73">
-        <f t="shared" si="1"/>
+      <c r="J73">
+        <f t="shared" si="2"/>
         <v>30.71</v>
       </c>
-      <c r="M73" s="3">
+      <c r="N73" s="3">
         <v>54</v>
       </c>
-      <c r="P73" s="3">
+      <c r="Q73" s="3">
         <v>8</v>
       </c>
-      <c r="Q73" s="3">
+      <c r="R73" s="3">
         <v>16.670000000000002</v>
       </c>
-      <c r="R73" s="3">
+      <c r="S73" s="3">
         <v>116.7</v>
       </c>
-      <c r="S73" s="3">
+      <c r="T73" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>70</v>
       </c>
@@ -3291,30 +3480,31 @@
       <c r="G74" s="3">
         <v>32.270000000000003</v>
       </c>
-      <c r="H74" s="3">
+      <c r="H74" s="3"/>
+      <c r="I74" s="3">
         <v>65.22</v>
       </c>
-      <c r="I74">
-        <f t="shared" si="1"/>
+      <c r="J74">
+        <f t="shared" si="2"/>
         <v>32.949999999999996</v>
       </c>
-      <c r="M74" s="3">
+      <c r="N74" s="3">
         <v>54</v>
       </c>
-      <c r="P74" s="3">
+      <c r="Q74" s="3">
         <v>6.33</v>
       </c>
-      <c r="Q74" s="3">
+      <c r="R74" s="3">
         <v>19.670000000000002</v>
       </c>
-      <c r="R74" s="3">
+      <c r="S74" s="3">
         <v>117.53</v>
       </c>
-      <c r="S74" s="3">
+      <c r="T74" s="3">
         <v>50.79</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>71</v>
       </c>
@@ -3334,30 +3524,31 @@
       <c r="G75" s="3">
         <v>27.12</v>
       </c>
-      <c r="H75" s="3">
+      <c r="H75" s="3"/>
+      <c r="I75" s="3">
         <v>49.24</v>
       </c>
-      <c r="I75">
-        <f t="shared" si="1"/>
+      <c r="J75">
+        <f t="shared" si="2"/>
         <v>22.12</v>
       </c>
-      <c r="M75" s="3">
+      <c r="N75" s="3">
         <v>51.67</v>
       </c>
-      <c r="P75" s="3">
+      <c r="Q75" s="3">
         <v>7</v>
       </c>
-      <c r="Q75" s="3">
+      <c r="R75" s="3">
         <v>13</v>
       </c>
-      <c r="R75" s="3">
+      <c r="S75" s="3">
         <v>116.8</v>
       </c>
-      <c r="S75" s="3">
+      <c r="T75" s="3">
         <v>45.96</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>72</v>
       </c>
@@ -3377,30 +3568,31 @@
       <c r="G76" s="3">
         <v>33.979999999999997</v>
       </c>
-      <c r="H76" s="3">
+      <c r="H76" s="3"/>
+      <c r="I76" s="3">
         <v>65.78</v>
       </c>
-      <c r="I76">
-        <f t="shared" si="1"/>
+      <c r="J76">
+        <f t="shared" si="2"/>
         <v>31.800000000000004</v>
       </c>
-      <c r="M76" s="3">
+      <c r="N76" s="3">
         <v>51.33</v>
       </c>
-      <c r="P76" s="3">
+      <c r="Q76" s="3">
         <v>8.67</v>
       </c>
-      <c r="Q76" s="3">
+      <c r="R76" s="3">
         <v>20.67</v>
       </c>
-      <c r="R76" s="3">
+      <c r="S76" s="3">
         <v>120.95</v>
       </c>
-      <c r="S76" s="3">
+      <c r="T76" s="3">
         <v>46.91</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>73</v>
       </c>
@@ -3420,30 +3612,31 @@
       <c r="G77" s="3">
         <v>31.38</v>
       </c>
-      <c r="H77" s="3">
+      <c r="H77" s="3"/>
+      <c r="I77" s="3">
         <v>60.02</v>
       </c>
-      <c r="I77">
-        <f t="shared" si="1"/>
+      <c r="J77">
+        <f t="shared" si="2"/>
         <v>28.640000000000004</v>
       </c>
-      <c r="M77" s="3">
+      <c r="N77" s="3">
         <v>51</v>
       </c>
-      <c r="P77" s="3">
+      <c r="Q77" s="3">
         <v>6</v>
       </c>
-      <c r="Q77" s="3">
+      <c r="R77" s="3">
         <v>16</v>
       </c>
-      <c r="R77" s="3">
+      <c r="S77" s="3">
         <v>119.07</v>
       </c>
-      <c r="S77" s="3">
+      <c r="T77" s="3">
         <v>46.91</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>74</v>
       </c>
@@ -3463,30 +3656,31 @@
       <c r="G78" s="3">
         <v>22.63</v>
       </c>
-      <c r="H78" s="3">
+      <c r="H78" s="3"/>
+      <c r="I78" s="3">
         <v>41.72</v>
       </c>
-      <c r="I78">
-        <f t="shared" si="1"/>
+      <c r="J78">
+        <f t="shared" si="2"/>
         <v>19.09</v>
       </c>
-      <c r="M78" s="3">
+      <c r="N78" s="3">
         <v>52.33</v>
       </c>
-      <c r="P78" s="3">
+      <c r="Q78" s="3">
         <v>9</v>
       </c>
-      <c r="Q78" s="3">
+      <c r="R78" s="3">
         <v>14.33</v>
       </c>
-      <c r="R78" s="3">
+      <c r="S78" s="3">
         <v>116.23</v>
       </c>
-      <c r="S78" s="3">
+      <c r="T78" s="3">
         <v>37.659999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>75</v>
       </c>
@@ -3506,30 +3700,31 @@
       <c r="G79" s="3">
         <v>32.58</v>
       </c>
-      <c r="H79" s="3">
+      <c r="H79" s="3"/>
+      <c r="I79" s="3">
         <v>64.73</v>
       </c>
-      <c r="I79">
-        <f t="shared" si="1"/>
+      <c r="J79">
+        <f t="shared" si="2"/>
         <v>32.150000000000006</v>
       </c>
-      <c r="M79" s="3">
+      <c r="N79" s="3">
         <v>51.67</v>
       </c>
-      <c r="P79" s="3">
+      <c r="Q79" s="3">
         <v>8.67</v>
       </c>
-      <c r="Q79" s="3">
+      <c r="R79" s="3">
         <v>13</v>
       </c>
-      <c r="R79" s="3">
+      <c r="S79" s="3">
         <v>117.1</v>
       </c>
-      <c r="S79" s="3">
+      <c r="T79" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>76</v>
       </c>
@@ -3549,30 +3744,31 @@
       <c r="G80" s="3">
         <v>27</v>
       </c>
-      <c r="H80" s="3">
+      <c r="H80" s="3"/>
+      <c r="I80" s="3">
         <v>51.83</v>
       </c>
-      <c r="I80">
-        <f t="shared" si="1"/>
+      <c r="J80">
+        <f t="shared" si="2"/>
         <v>24.83</v>
       </c>
-      <c r="M80" s="3">
+      <c r="N80" s="3">
         <v>54</v>
       </c>
-      <c r="P80" s="3">
+      <c r="Q80" s="3">
         <v>5.67</v>
       </c>
-      <c r="Q80" s="3">
+      <c r="R80" s="3">
         <v>16</v>
       </c>
-      <c r="R80" s="3">
+      <c r="S80" s="3">
         <v>119</v>
       </c>
-      <c r="S80" s="3">
+      <c r="T80" s="3">
         <v>42.12</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>77</v>
       </c>
@@ -3592,30 +3788,31 @@
       <c r="G81" s="3">
         <v>23.69</v>
       </c>
-      <c r="H81" s="3">
+      <c r="H81" s="3"/>
+      <c r="I81" s="3">
         <v>43.4</v>
       </c>
-      <c r="I81">
-        <f t="shared" si="1"/>
+      <c r="J81">
+        <f t="shared" si="2"/>
         <v>19.709999999999997</v>
       </c>
-      <c r="M81" s="3">
+      <c r="N81" s="3">
         <v>53.67</v>
       </c>
-      <c r="P81" s="3">
+      <c r="Q81" s="3">
         <v>6</v>
       </c>
-      <c r="Q81" s="3">
+      <c r="R81" s="3">
         <v>9</v>
       </c>
-      <c r="R81" s="3">
+      <c r="S81" s="3">
         <v>114.92</v>
       </c>
-      <c r="S81" s="3">
+      <c r="T81" s="3">
         <v>38.44</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>78</v>
       </c>
@@ -3635,30 +3832,31 @@
       <c r="G82" s="3">
         <v>33.26</v>
       </c>
-      <c r="H82" s="3">
+      <c r="H82" s="3"/>
+      <c r="I82" s="3">
         <v>54.95</v>
       </c>
-      <c r="I82">
-        <f t="shared" si="1"/>
+      <c r="J82">
+        <f t="shared" si="2"/>
         <v>21.690000000000005</v>
       </c>
-      <c r="M82" s="3">
+      <c r="N82" s="3">
         <v>50.67</v>
       </c>
-      <c r="P82" s="3">
+      <c r="Q82" s="3">
         <v>9</v>
       </c>
-      <c r="Q82" s="3">
+      <c r="R82" s="3">
         <v>12.67</v>
       </c>
-      <c r="R82" s="3">
+      <c r="S82" s="3">
         <v>117.8</v>
       </c>
-      <c r="S82" s="3">
+      <c r="T82" s="3">
         <v>43.09</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>79</v>
       </c>
@@ -3678,26 +3876,27 @@
       <c r="G83" s="3">
         <v>29.46</v>
       </c>
-      <c r="H83" s="3">
+      <c r="H83" s="3"/>
+      <c r="I83" s="3">
         <v>52.77</v>
       </c>
-      <c r="I83">
-        <f t="shared" si="1"/>
+      <c r="J83">
+        <f t="shared" si="2"/>
         <v>23.310000000000002</v>
       </c>
-      <c r="M83" s="3">
+      <c r="N83" s="3">
         <v>54.67</v>
       </c>
-      <c r="P83" s="3">
+      <c r="Q83" s="3">
         <v>6</v>
       </c>
-      <c r="Q83" s="3">
+      <c r="R83" s="3">
         <v>18.329999999999998</v>
       </c>
-      <c r="R83" s="3">
+      <c r="S83" s="3">
         <v>118.27</v>
       </c>
-      <c r="S83" s="3">
+      <c r="T83" s="3">
         <v>41.16</v>
       </c>
     </row>
@@ -3710,11 +3909,1311 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A2:A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="1">
+        <f>DATE(2012,3,11)+C2</f>
+        <v>40989</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>23.7</v>
+      </c>
+      <c r="E2">
+        <v>78.8</v>
+      </c>
+      <c r="F2">
+        <v>102.5</v>
+      </c>
+      <c r="G2">
+        <v>23.7</v>
+      </c>
+      <c r="H2">
+        <v>2.4</v>
+      </c>
+      <c r="I2">
+        <v>6.1</v>
+      </c>
+      <c r="J2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="1">
+        <f t="shared" ref="B3:B14" si="0">DATE(2012,3,11)+C3</f>
+        <v>40994</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>13.3</v>
+      </c>
+      <c r="E3">
+        <v>89.1</v>
+      </c>
+      <c r="F3">
+        <v>102.5</v>
+      </c>
+      <c r="G3">
+        <v>13.4</v>
+      </c>
+      <c r="H3">
+        <v>2.7</v>
+      </c>
+      <c r="I3">
+        <v>6.4</v>
+      </c>
+      <c r="J3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" si="0"/>
+        <v>40997</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>97.5</v>
+      </c>
+      <c r="F4">
+        <v>102.5</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>1.7</v>
+      </c>
+      <c r="I4">
+        <v>6.3</v>
+      </c>
+      <c r="J4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>41004</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>21.7</v>
+      </c>
+      <c r="E5">
+        <v>80.8</v>
+      </c>
+      <c r="F5">
+        <v>102.5</v>
+      </c>
+      <c r="G5">
+        <v>21.7</v>
+      </c>
+      <c r="H5">
+        <v>3.1</v>
+      </c>
+      <c r="I5">
+        <v>5.2</v>
+      </c>
+      <c r="J5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>41012</v>
+      </c>
+      <c r="C6">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="E6">
+        <v>126.4</v>
+      </c>
+      <c r="F6">
+        <v>163.1</v>
+      </c>
+      <c r="G6">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="H6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>41018</v>
+      </c>
+      <c r="C7">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>33.1</v>
+      </c>
+      <c r="E7">
+        <v>130</v>
+      </c>
+      <c r="F7">
+        <v>163.1</v>
+      </c>
+      <c r="G7">
+        <v>33.1</v>
+      </c>
+      <c r="H7">
+        <v>5.5</v>
+      </c>
+      <c r="I7">
+        <v>5.6</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>41022</v>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+      <c r="D8">
+        <v>22.1</v>
+      </c>
+      <c r="E8">
+        <v>141</v>
+      </c>
+      <c r="F8">
+        <v>163.1</v>
+      </c>
+      <c r="G8">
+        <v>22.1</v>
+      </c>
+      <c r="H8">
+        <v>5.5</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>41026</v>
+      </c>
+      <c r="C9">
+        <v>47</v>
+      </c>
+      <c r="D9">
+        <v>22.1</v>
+      </c>
+      <c r="E9">
+        <v>141</v>
+      </c>
+      <c r="F9">
+        <v>163.1</v>
+      </c>
+      <c r="G9">
+        <v>22.1</v>
+      </c>
+      <c r="H9">
+        <v>5.5</v>
+      </c>
+      <c r="I9">
+        <v>6.2</v>
+      </c>
+      <c r="J9">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>41029</v>
+      </c>
+      <c r="C10">
+        <v>50</v>
+      </c>
+      <c r="D10">
+        <v>25.6</v>
+      </c>
+      <c r="E10">
+        <v>137.5</v>
+      </c>
+      <c r="F10">
+        <v>163.1</v>
+      </c>
+      <c r="G10">
+        <v>25.6</v>
+      </c>
+      <c r="H10">
+        <v>8.5</v>
+      </c>
+      <c r="I10">
+        <v>5.4</v>
+      </c>
+      <c r="J10">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>41032</v>
+      </c>
+      <c r="C11">
+        <v>53</v>
+      </c>
+      <c r="D11">
+        <v>20.2</v>
+      </c>
+      <c r="E11">
+        <v>142.9</v>
+      </c>
+      <c r="F11">
+        <v>163.1</v>
+      </c>
+      <c r="G11">
+        <v>20.2</v>
+      </c>
+      <c r="H11">
+        <v>6.7</v>
+      </c>
+      <c r="I11">
+        <v>5.9</v>
+      </c>
+      <c r="J11">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>41041</v>
+      </c>
+      <c r="C12">
+        <v>62</v>
+      </c>
+      <c r="D12">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="E12">
+        <v>129.4</v>
+      </c>
+      <c r="F12">
+        <v>163.1</v>
+      </c>
+      <c r="G12">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="H12">
+        <v>3.7</v>
+      </c>
+      <c r="I12">
+        <v>6.5</v>
+      </c>
+      <c r="J12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>41049</v>
+      </c>
+      <c r="C13">
+        <v>70</v>
+      </c>
+      <c r="D13">
+        <v>30.2</v>
+      </c>
+      <c r="E13">
+        <v>132.9</v>
+      </c>
+      <c r="F13">
+        <v>163.1</v>
+      </c>
+      <c r="G13">
+        <v>30.2</v>
+      </c>
+      <c r="H13">
+        <v>3.8</v>
+      </c>
+      <c r="I13">
+        <v>5.6</v>
+      </c>
+      <c r="J13">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>41053</v>
+      </c>
+      <c r="C14">
+        <v>74</v>
+      </c>
+      <c r="D14">
+        <v>12.3</v>
+      </c>
+      <c r="E14">
+        <v>150.80000000000001</v>
+      </c>
+      <c r="F14">
+        <v>163.1</v>
+      </c>
+      <c r="G14">
+        <v>12.3</v>
+      </c>
+      <c r="H14">
+        <v>3.1</v>
+      </c>
+      <c r="I14">
+        <v>5.3</v>
+      </c>
+      <c r="J14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>77</v>
+      </c>
+      <c r="C2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>81</v>
+      </c>
+      <c r="C3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>85</v>
+      </c>
+      <c r="C4">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>83</v>
+      </c>
+      <c r="C6">
+        <v>145</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>90</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>56</v>
+      </c>
+      <c r="C10">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>58</v>
+      </c>
+      <c r="C11">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>61</v>
+      </c>
+      <c r="C12">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>62</v>
+      </c>
+      <c r="C13">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>57</v>
+      </c>
+      <c r="C14">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1">
+        <v>40531</v>
+      </c>
+      <c r="C2">
+        <v>0.100411</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D39" si="0">LN(1-C2)/-0.65</f>
+        <v>0.16279582558226338</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1">
+        <v>40543</v>
+      </c>
+      <c r="C3">
+        <v>0.49978700000000004</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>1.0657250327264367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40554</v>
+      </c>
+      <c r="C4">
+        <v>0.80300700000000003</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2.4993647444159759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1">
+        <v>40564</v>
+      </c>
+      <c r="C5">
+        <v>0.90274399999999999</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3.5852440026594521</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>40574</v>
+      </c>
+      <c r="C6">
+        <v>0.95303899999999997</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>4.7052889368770998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1">
+        <v>40584</v>
+      </c>
+      <c r="C7">
+        <v>0.95683200000000002</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4.8348550753181421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1">
+        <v>40594</v>
+      </c>
+      <c r="C8">
+        <v>0.60590699999999997</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.4325667029665659</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1">
+        <v>40531</v>
+      </c>
+      <c r="C9">
+        <v>0.10197300000000001</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.16546945279506198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1">
+        <v>40543</v>
+      </c>
+      <c r="C10">
+        <v>0.50231199999999998</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.0735106220284432</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1">
+        <v>40554</v>
+      </c>
+      <c r="C11">
+        <v>0.80115599999999998</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2.4849764327404271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1">
+        <v>40564</v>
+      </c>
+      <c r="C12">
+        <v>0.89999499999999999</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>3.5423616834523135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1">
+        <v>40574</v>
+      </c>
+      <c r="C13">
+        <v>0.90608599999999995</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3.6390397063073214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1">
+        <v>40584</v>
+      </c>
+      <c r="C14">
+        <v>0.90347100000000002</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>3.5967873809984794</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="1">
+        <v>40594</v>
+      </c>
+      <c r="C15">
+        <v>0.60232399999999997</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1.4186425778225658</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1">
+        <v>40531</v>
+      </c>
+      <c r="C16">
+        <v>0.100436</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.16283858074367979</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1">
+        <v>40543</v>
+      </c>
+      <c r="C17">
+        <v>0.45323200000000002</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.92881645870226348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1">
+        <v>40554</v>
+      </c>
+      <c r="C18">
+        <v>0.70411600000000008</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1.8735196820917912</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1">
+        <v>40564</v>
+      </c>
+      <c r="C19">
+        <v>0.80382699999999996</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>2.5057820861531415</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1">
+        <v>40574</v>
+      </c>
+      <c r="C20">
+        <v>0.85994799999999993</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3.0242176873291071</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="1">
+        <v>40584</v>
+      </c>
+      <c r="C21">
+        <v>0.80850300000000008</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>2.5428971327392174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="1">
+        <v>40594</v>
+      </c>
+      <c r="C22">
+        <v>0.55935299999999999</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>1.2607864270523148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="1">
+        <v>40531</v>
+      </c>
+      <c r="C23">
+        <v>0.10513400000000001</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>0.17089429628758651</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="1">
+        <v>40543</v>
+      </c>
+      <c r="C24">
+        <v>0.40342300000000003</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0.79468762990480768</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="1">
+        <v>40554</v>
+      </c>
+      <c r="C25">
+        <v>0.60146699999999997</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1.4153307286783807</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1">
+        <v>40564</v>
+      </c>
+      <c r="C26">
+        <v>0.704156</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1.8737276778656335</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1">
+        <v>40574</v>
+      </c>
+      <c r="C27">
+        <v>0.70171099999999997</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1.861065328876798</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>40584</v>
+      </c>
+      <c r="C28">
+        <v>0.400978</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0.78839531332513868</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="6">
+        <v>39692</v>
+      </c>
+      <c r="C29">
+        <v>0.32997599999999999</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0.61606422514331682</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="6">
+        <v>39702</v>
+      </c>
+      <c r="C30">
+        <v>0.61774600000000002</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>1.4794922613414281</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="6">
+        <v>39712</v>
+      </c>
+      <c r="C31">
+        <v>0.69256600000000001</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>1.8146074598755551</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="6">
+        <v>39722</v>
+      </c>
+      <c r="C32">
+        <v>0.57362099999999994</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1.3114256259603951</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="6">
+        <v>39732</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="6">
+        <v>39692</v>
+      </c>
+      <c r="C34">
+        <v>0.37985599999999997</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>0.73508241514801897</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="6">
+        <v>39702</v>
+      </c>
+      <c r="C35">
+        <v>0.58896900000000008</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>1.367825602368508</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="6">
+        <v>39712</v>
+      </c>
+      <c r="C36">
+        <v>0.65995199999999998</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>1.6594899921012336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="6">
+        <v>39722</v>
+      </c>
+      <c r="C37">
+        <v>0.70599500000000004</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>1.883320776900536</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" s="6">
+        <v>39732</v>
+      </c>
+      <c r="C38">
+        <v>0.72134299999999996</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>1.9658056064037499</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="6">
+        <v>39742</v>
+      </c>
+      <c r="C39">
+        <v>0.68489199999999995</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>1.7766766796549629</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4582,7 +6081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -4975,7 +6474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D148"/>
   <sheetViews>
@@ -7212,12 +8711,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:K8"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7825,7 +9324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -8317,7 +9816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
@@ -8893,492 +10392,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A2:A14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" t="s">
-        <v>136</v>
-      </c>
-      <c r="F1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H1" t="s">
-        <v>139</v>
-      </c>
-      <c r="I1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" s="1">
-        <f>DATE(2012,3,11)+C2</f>
-        <v>40989</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>23.7</v>
-      </c>
-      <c r="E2">
-        <v>78.8</v>
-      </c>
-      <c r="F2">
-        <v>102.5</v>
-      </c>
-      <c r="G2">
-        <v>23.7</v>
-      </c>
-      <c r="H2">
-        <v>2.4</v>
-      </c>
-      <c r="I2">
-        <v>6.1</v>
-      </c>
-      <c r="J2">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B3" s="1">
-        <f t="shared" ref="B3:B14" si="0">DATE(2012,3,11)+C3</f>
-        <v>40994</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>13.3</v>
-      </c>
-      <c r="E3">
-        <v>89.1</v>
-      </c>
-      <c r="F3">
-        <v>102.5</v>
-      </c>
-      <c r="G3">
-        <v>13.4</v>
-      </c>
-      <c r="H3">
-        <v>2.7</v>
-      </c>
-      <c r="I3">
-        <v>6.4</v>
-      </c>
-      <c r="J3">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B4" s="1">
-        <f t="shared" si="0"/>
-        <v>40997</v>
-      </c>
-      <c r="C4">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>97.5</v>
-      </c>
-      <c r="F4">
-        <v>102.5</v>
-      </c>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="H4">
-        <v>1.7</v>
-      </c>
-      <c r="I4">
-        <v>6.3</v>
-      </c>
-      <c r="J4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="1">
-        <f t="shared" si="0"/>
-        <v>41004</v>
-      </c>
-      <c r="C5">
-        <v>25</v>
-      </c>
-      <c r="D5">
-        <v>21.7</v>
-      </c>
-      <c r="E5">
-        <v>80.8</v>
-      </c>
-      <c r="F5">
-        <v>102.5</v>
-      </c>
-      <c r="G5">
-        <v>21.7</v>
-      </c>
-      <c r="H5">
-        <v>3.1</v>
-      </c>
-      <c r="I5">
-        <v>5.2</v>
-      </c>
-      <c r="J5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B6" s="1">
-        <f t="shared" si="0"/>
-        <v>41012</v>
-      </c>
-      <c r="C6">
-        <v>33</v>
-      </c>
-      <c r="D6">
-        <v>36.700000000000003</v>
-      </c>
-      <c r="E6">
-        <v>126.4</v>
-      </c>
-      <c r="F6">
-        <v>163.1</v>
-      </c>
-      <c r="G6">
-        <v>36.700000000000003</v>
-      </c>
-      <c r="H6">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="I6">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="J6">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" s="1">
-        <f t="shared" si="0"/>
-        <v>41018</v>
-      </c>
-      <c r="C7">
-        <v>39</v>
-      </c>
-      <c r="D7">
-        <v>33.1</v>
-      </c>
-      <c r="E7">
-        <v>130</v>
-      </c>
-      <c r="F7">
-        <v>163.1</v>
-      </c>
-      <c r="G7">
-        <v>33.1</v>
-      </c>
-      <c r="H7">
-        <v>5.5</v>
-      </c>
-      <c r="I7">
-        <v>5.6</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" s="1">
-        <f t="shared" si="0"/>
-        <v>41022</v>
-      </c>
-      <c r="C8">
-        <v>43</v>
-      </c>
-      <c r="D8">
-        <v>22.1</v>
-      </c>
-      <c r="E8">
-        <v>141</v>
-      </c>
-      <c r="F8">
-        <v>163.1</v>
-      </c>
-      <c r="G8">
-        <v>22.1</v>
-      </c>
-      <c r="H8">
-        <v>5.5</v>
-      </c>
-      <c r="I8">
-        <v>7</v>
-      </c>
-      <c r="J8">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>142</v>
-      </c>
-      <c r="B9" s="1">
-        <f t="shared" si="0"/>
-        <v>41026</v>
-      </c>
-      <c r="C9">
-        <v>47</v>
-      </c>
-      <c r="D9">
-        <v>22.1</v>
-      </c>
-      <c r="E9">
-        <v>141</v>
-      </c>
-      <c r="F9">
-        <v>163.1</v>
-      </c>
-      <c r="G9">
-        <v>22.1</v>
-      </c>
-      <c r="H9">
-        <v>5.5</v>
-      </c>
-      <c r="I9">
-        <v>6.2</v>
-      </c>
-      <c r="J9">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>142</v>
-      </c>
-      <c r="B10" s="1">
-        <f t="shared" si="0"/>
-        <v>41029</v>
-      </c>
-      <c r="C10">
-        <v>50</v>
-      </c>
-      <c r="D10">
-        <v>25.6</v>
-      </c>
-      <c r="E10">
-        <v>137.5</v>
-      </c>
-      <c r="F10">
-        <v>163.1</v>
-      </c>
-      <c r="G10">
-        <v>25.6</v>
-      </c>
-      <c r="H10">
-        <v>8.5</v>
-      </c>
-      <c r="I10">
-        <v>5.4</v>
-      </c>
-      <c r="J10">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="1">
-        <f t="shared" si="0"/>
-        <v>41032</v>
-      </c>
-      <c r="C11">
-        <v>53</v>
-      </c>
-      <c r="D11">
-        <v>20.2</v>
-      </c>
-      <c r="E11">
-        <v>142.9</v>
-      </c>
-      <c r="F11">
-        <v>163.1</v>
-      </c>
-      <c r="G11">
-        <v>20.2</v>
-      </c>
-      <c r="H11">
-        <v>6.7</v>
-      </c>
-      <c r="I11">
-        <v>5.9</v>
-      </c>
-      <c r="J11">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" si="0"/>
-        <v>41041</v>
-      </c>
-      <c r="C12">
-        <v>62</v>
-      </c>
-      <c r="D12">
-        <v>33.700000000000003</v>
-      </c>
-      <c r="E12">
-        <v>129.4</v>
-      </c>
-      <c r="F12">
-        <v>163.1</v>
-      </c>
-      <c r="G12">
-        <v>33.700000000000003</v>
-      </c>
-      <c r="H12">
-        <v>3.7</v>
-      </c>
-      <c r="I12">
-        <v>6.5</v>
-      </c>
-      <c r="J12">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>142</v>
-      </c>
-      <c r="B13" s="1">
-        <f t="shared" si="0"/>
-        <v>41049</v>
-      </c>
-      <c r="C13">
-        <v>70</v>
-      </c>
-      <c r="D13">
-        <v>30.2</v>
-      </c>
-      <c r="E13">
-        <v>132.9</v>
-      </c>
-      <c r="F13">
-        <v>163.1</v>
-      </c>
-      <c r="G13">
-        <v>30.2</v>
-      </c>
-      <c r="H13">
-        <v>3.8</v>
-      </c>
-      <c r="I13">
-        <v>5.6</v>
-      </c>
-      <c r="J13">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B14" s="1">
-        <f t="shared" si="0"/>
-        <v>41053</v>
-      </c>
-      <c r="C14">
-        <v>74</v>
-      </c>
-      <c r="D14">
-        <v>12.3</v>
-      </c>
-      <c r="E14">
-        <v>150.80000000000001</v>
-      </c>
-      <c r="F14">
-        <v>163.1</v>
-      </c>
-      <c r="G14">
-        <v>12.3</v>
-      </c>
-      <c r="H14">
-        <v>3.1</v>
-      </c>
-      <c r="I14">
-        <v>5.3</v>
-      </c>
-      <c r="J14">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new dataset to Tef validation set
</commit_message>
<xml_diff>
--- a/Prototypes/Teff/Observed.xlsx
+++ b/Prototypes/Teff/Observed.xlsx
@@ -28,7 +28,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="O27" authorId="0" shapeId="0">
+    <comment ref="P27" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O64" authorId="0" shapeId="0">
+    <comment ref="P64" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O67" authorId="0" shapeId="0">
+    <comment ref="P67" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="165">
   <si>
     <t>SimulationName</t>
   </si>
@@ -634,6 +634,54 @@
   </si>
   <si>
     <t>Teff.Leaf.LAI</t>
+  </si>
+  <si>
+    <t>Mekelle2004N0</t>
+  </si>
+  <si>
+    <t>Mekelle2004N1</t>
+  </si>
+  <si>
+    <t>Mekelle2004N2</t>
+  </si>
+  <si>
+    <t>HI</t>
+  </si>
+  <si>
+    <t>Mekelle2004N0Split</t>
+  </si>
+  <si>
+    <t>Mekelle2004N1Split</t>
+  </si>
+  <si>
+    <t>Mekelle2004N2Split</t>
+  </si>
+  <si>
+    <t>Mekelle2005N0</t>
+  </si>
+  <si>
+    <t>Mekelle2005N1</t>
+  </si>
+  <si>
+    <t>Mekelle2005N2</t>
+  </si>
+  <si>
+    <t>Mekelle2005N0Split</t>
+  </si>
+  <si>
+    <t>Mekelle2005N1Split</t>
+  </si>
+  <si>
+    <t>Mekelle2005N2Split</t>
+  </si>
+  <si>
+    <t>StrawNConc</t>
+  </si>
+  <si>
+    <t>GrainPerPanicle</t>
+  </si>
+  <si>
+    <t>PPSM</t>
   </si>
 </sst>
 </file>
@@ -1234,11 +1282,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="438485656"/>
-        <c:axId val="438486048"/>
+        <c:axId val="275180120"/>
+        <c:axId val="275180512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="438485656"/>
+        <c:axId val="275180120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1248,12 +1296,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="438486048"/>
+        <c:crossAx val="275180512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438486048"/>
+        <c:axId val="275180512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="40"/>
@@ -1265,7 +1313,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="438485656"/>
+        <c:crossAx val="275180120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1500,11 +1548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="438487616"/>
-        <c:axId val="438488008"/>
+        <c:axId val="275182080"/>
+        <c:axId val="277052808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="438487616"/>
+        <c:axId val="275182080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,12 +1562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="438488008"/>
+        <c:crossAx val="277052808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="438488008"/>
+        <c:axId val="277052808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1530,7 +1578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="438487616"/>
+        <c:crossAx val="275182080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1908,24 +1956,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T83"/>
+  <dimension ref="A1:X95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <pane xSplit="4416" ySplit="600" topLeftCell="B77" activePane="bottomRight"/>
+      <selection sqref="A1:XFD1"/>
+      <selection pane="topRight" activeCell="X1" sqref="X1"/>
+      <selection pane="bottomLeft" activeCell="A95" sqref="A95"/>
+      <selection pane="bottomRight" activeCell="X84" sqref="X84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1957,37 +2009,49 @@
         <v>85</v>
       </c>
       <c r="K1" t="s">
+        <v>162</v>
+      </c>
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>61</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>80</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>81</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>82</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V1" t="s">
+        <v>152</v>
+      </c>
+      <c r="W1" t="s">
+        <v>163</v>
+      </c>
+      <c r="X1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -2018,17 +2082,17 @@
         <f>I2-G2</f>
         <v>0.52</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>68.7</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>76.7</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -2058,17 +2122,17 @@
         <f t="shared" ref="J3:J11" si="1">I3-G3</f>
         <v>0.96999999999999975</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>72</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>81.3</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>142.30000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2098,17 +2162,17 @@
         <f t="shared" si="1"/>
         <v>1.37</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>76</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>85</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>146.30000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2138,17 +2202,17 @@
         <f t="shared" si="1"/>
         <v>1.8699999999999992</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>80.7</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>90</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2178,17 +2242,17 @@
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>74</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>83.3</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2218,21 +2282,21 @@
         <f t="shared" si="1"/>
         <v>4.58</v>
       </c>
-      <c r="L7">
-        <f>E7/10/M7</f>
+      <c r="M7">
+        <f>E7/10/N7</f>
         <v>84440</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>2.5000000000000001E-4</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>56.3</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>85.7</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2262,21 +2326,21 @@
         <f t="shared" si="1"/>
         <v>5.58</v>
       </c>
-      <c r="L8">
-        <f>E8/10/M8</f>
+      <c r="M8">
+        <f>E8/10/N8</f>
         <v>104851.85185185185</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>2.7E-4</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>58</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>88.3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2306,21 +2370,21 @@
         <f t="shared" si="1"/>
         <v>8.0000000000000018</v>
       </c>
-      <c r="L9">
-        <f>E9/10/M9</f>
+      <c r="M9">
+        <f>E9/10/N9</f>
         <v>109032.25806451612</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>3.1E-4</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>60.7</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2350,21 +2414,21 @@
         <f t="shared" si="1"/>
         <v>11.36</v>
       </c>
-      <c r="L10">
-        <f>E10/10/M10</f>
+      <c r="M10">
+        <f>E10/10/N10</f>
         <v>98400</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>3.5E-4</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>61.7</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <v>91.7</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2394,21 +2458,21 @@
         <f t="shared" si="1"/>
         <v>6.0900000000000007</v>
       </c>
-      <c r="L11">
-        <f>E11/10/M11</f>
+      <c r="M11">
+        <f>E11/10/N11</f>
         <v>104214.28571428572</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>2.7999999999999998E-4</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>57.3</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>88.7</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2419,7 +2483,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -2430,7 +2494,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -2441,7 +2505,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -2452,7 +2516,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
@@ -2463,7 +2527,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
@@ -2474,7 +2538,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
@@ -2485,7 +2549,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
@@ -2496,7 +2560,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
@@ -2507,7 +2571,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -2518,7 +2582,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -2529,7 +2593,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
@@ -2540,7 +2604,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
@@ -2551,7 +2615,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>47</v>
       </c>
@@ -2562,7 +2626,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
@@ -2573,7 +2637,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
@@ -2583,14 +2647,14 @@
       <c r="E27">
         <v>285</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>56</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -2601,7 +2665,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
@@ -2612,7 +2676,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -2623,7 +2687,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>28</v>
       </c>
@@ -2634,7 +2698,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -2851,7 +2915,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>91</v>
       </c>
@@ -2868,7 +2932,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>92</v>
       </c>
@@ -2885,7 +2949,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>93</v>
       </c>
@@ -2902,7 +2966,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>94</v>
       </c>
@@ -2919,7 +2983,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>95</v>
       </c>
@@ -2936,7 +3000,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>96</v>
       </c>
@@ -2953,7 +3017,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>97</v>
       </c>
@@ -2970,7 +3034,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>98</v>
       </c>
@@ -2987,7 +3051,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>99</v>
       </c>
@@ -3004,7 +3068,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>100</v>
       </c>
@@ -3021,7 +3085,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>101</v>
       </c>
@@ -3038,7 +3102,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>53</v>
       </c>
@@ -3055,7 +3119,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>54</v>
       </c>
@@ -3072,7 +3136,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>55</v>
       </c>
@@ -3089,7 +3153,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>56</v>
       </c>
@@ -3106,7 +3170,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>57</v>
       </c>
@@ -3122,15 +3186,15 @@
       <c r="F64">
         <v>567</v>
       </c>
-      <c r="O64">
+      <c r="P64">
         <f>46+8</f>
         <v>54</v>
       </c>
-      <c r="P64">
+      <c r="Q64">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>58</v>
       </c>
@@ -3147,7 +3211,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>59</v>
       </c>
@@ -3164,7 +3228,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>60</v>
       </c>
@@ -3180,15 +3244,15 @@
       <c r="F67">
         <v>440</v>
       </c>
-      <c r="O67">
+      <c r="P67">
         <f>44+8</f>
         <v>52</v>
       </c>
-      <c r="P67">
+      <c r="Q67">
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>64</v>
       </c>
@@ -3214,33 +3278,33 @@
         <f t="shared" ref="J68:J83" si="2">I68-G68</f>
         <v>13.2</v>
       </c>
-      <c r="L68">
-        <f>E12/10/M68</f>
+      <c r="M68">
+        <f>E12/10/N68</f>
         <v>100831.60083160082</v>
       </c>
-      <c r="M68">
+      <c r="N68">
         <v>2.8860000000000002E-4</v>
       </c>
-      <c r="N68">
+      <c r="O68">
         <v>48</v>
       </c>
-      <c r="P68">
+      <c r="Q68">
         <v>84.8</v>
       </c>
-      <c r="Q68">
+      <c r="R68">
         <v>5.47</v>
       </c>
-      <c r="R68">
+      <c r="S68">
         <v>7.73</v>
       </c>
-      <c r="S68">
+      <c r="T68">
         <v>95.75</v>
       </c>
-      <c r="T68">
+      <c r="U68">
         <v>28.85</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>65</v>
       </c>
@@ -3268,23 +3332,23 @@
         <f t="shared" si="2"/>
         <v>21.71</v>
       </c>
-      <c r="N69" s="3">
+      <c r="O69" s="3">
         <v>49.33</v>
       </c>
-      <c r="Q69" s="3">
+      <c r="R69" s="3">
         <v>4.67</v>
       </c>
-      <c r="R69" s="3">
+      <c r="S69" s="3">
         <v>11.33</v>
       </c>
-      <c r="S69" s="3">
+      <c r="T69" s="3">
         <v>112.58</v>
       </c>
-      <c r="T69" s="3">
+      <c r="U69" s="3">
         <v>34.43</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
@@ -3312,23 +3376,23 @@
         <f t="shared" si="2"/>
         <v>20.7</v>
       </c>
-      <c r="N70" s="3">
+      <c r="O70" s="3">
         <v>53.33</v>
       </c>
-      <c r="Q70" s="3">
+      <c r="R70" s="3">
         <v>5.33</v>
       </c>
-      <c r="R70" s="3">
+      <c r="S70" s="3">
         <v>17.329999999999998</v>
       </c>
-      <c r="S70" s="3">
+      <c r="T70" s="3">
         <v>113.25</v>
       </c>
-      <c r="T70" s="3">
+      <c r="U70" s="3">
         <v>36.44</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
@@ -3356,23 +3420,23 @@
         <f t="shared" si="2"/>
         <v>30.640000000000004</v>
       </c>
-      <c r="N71" s="3">
+      <c r="O71" s="3">
         <v>52</v>
       </c>
-      <c r="Q71" s="3">
+      <c r="R71" s="3">
         <v>7.33</v>
       </c>
-      <c r="R71" s="3">
+      <c r="S71" s="3">
         <v>17</v>
       </c>
-      <c r="S71" s="3">
+      <c r="T71" s="3">
         <v>112.22</v>
       </c>
-      <c r="T71" s="3">
+      <c r="U71" s="3">
         <v>47.88</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>68</v>
       </c>
@@ -3400,23 +3464,23 @@
         <f t="shared" si="2"/>
         <v>23.11</v>
       </c>
-      <c r="N72" s="3">
+      <c r="O72" s="3">
         <v>52.67</v>
       </c>
-      <c r="Q72" s="3">
+      <c r="R72" s="3">
         <v>6</v>
       </c>
-      <c r="R72" s="3">
+      <c r="S72" s="3">
         <v>15</v>
       </c>
-      <c r="S72" s="3">
+      <c r="T72" s="3">
         <v>113.41</v>
       </c>
-      <c r="T72" s="3">
+      <c r="U72" s="3">
         <v>41.15</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>69</v>
       </c>
@@ -3444,23 +3508,23 @@
         <f t="shared" si="2"/>
         <v>30.71</v>
       </c>
-      <c r="N73" s="3">
+      <c r="O73" s="3">
         <v>54</v>
       </c>
-      <c r="Q73" s="3">
+      <c r="R73" s="3">
         <v>8</v>
       </c>
-      <c r="R73" s="3">
+      <c r="S73" s="3">
         <v>16.670000000000002</v>
       </c>
-      <c r="S73" s="3">
+      <c r="T73" s="3">
         <v>116.7</v>
       </c>
-      <c r="T73" s="3">
+      <c r="U73" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>70</v>
       </c>
@@ -3488,23 +3552,23 @@
         <f t="shared" si="2"/>
         <v>32.949999999999996</v>
       </c>
-      <c r="N74" s="3">
+      <c r="O74" s="3">
         <v>54</v>
       </c>
-      <c r="Q74" s="3">
+      <c r="R74" s="3">
         <v>6.33</v>
       </c>
-      <c r="R74" s="3">
+      <c r="S74" s="3">
         <v>19.670000000000002</v>
       </c>
-      <c r="S74" s="3">
+      <c r="T74" s="3">
         <v>117.53</v>
       </c>
-      <c r="T74" s="3">
+      <c r="U74" s="3">
         <v>50.79</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>71</v>
       </c>
@@ -3532,23 +3596,23 @@
         <f t="shared" si="2"/>
         <v>22.12</v>
       </c>
-      <c r="N75" s="3">
+      <c r="O75" s="3">
         <v>51.67</v>
       </c>
-      <c r="Q75" s="3">
+      <c r="R75" s="3">
         <v>7</v>
       </c>
-      <c r="R75" s="3">
+      <c r="S75" s="3">
         <v>13</v>
       </c>
-      <c r="S75" s="3">
+      <c r="T75" s="3">
         <v>116.8</v>
       </c>
-      <c r="T75" s="3">
+      <c r="U75" s="3">
         <v>45.96</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>72</v>
       </c>
@@ -3576,23 +3640,23 @@
         <f t="shared" si="2"/>
         <v>31.800000000000004</v>
       </c>
-      <c r="N76" s="3">
+      <c r="O76" s="3">
         <v>51.33</v>
       </c>
-      <c r="Q76" s="3">
+      <c r="R76" s="3">
         <v>8.67</v>
       </c>
-      <c r="R76" s="3">
+      <c r="S76" s="3">
         <v>20.67</v>
       </c>
-      <c r="S76" s="3">
+      <c r="T76" s="3">
         <v>120.95</v>
       </c>
-      <c r="T76" s="3">
+      <c r="U76" s="3">
         <v>46.91</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>73</v>
       </c>
@@ -3620,23 +3684,23 @@
         <f t="shared" si="2"/>
         <v>28.640000000000004</v>
       </c>
-      <c r="N77" s="3">
+      <c r="O77" s="3">
         <v>51</v>
       </c>
-      <c r="Q77" s="3">
+      <c r="R77" s="3">
         <v>6</v>
       </c>
-      <c r="R77" s="3">
+      <c r="S77" s="3">
         <v>16</v>
       </c>
-      <c r="S77" s="3">
+      <c r="T77" s="3">
         <v>119.07</v>
       </c>
-      <c r="T77" s="3">
+      <c r="U77" s="3">
         <v>46.91</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>74</v>
       </c>
@@ -3664,23 +3728,23 @@
         <f t="shared" si="2"/>
         <v>19.09</v>
       </c>
-      <c r="N78" s="3">
+      <c r="O78" s="3">
         <v>52.33</v>
       </c>
-      <c r="Q78" s="3">
+      <c r="R78" s="3">
         <v>9</v>
       </c>
-      <c r="R78" s="3">
+      <c r="S78" s="3">
         <v>14.33</v>
       </c>
-      <c r="S78" s="3">
+      <c r="T78" s="3">
         <v>116.23</v>
       </c>
-      <c r="T78" s="3">
+      <c r="U78" s="3">
         <v>37.659999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>75</v>
       </c>
@@ -3708,23 +3772,23 @@
         <f t="shared" si="2"/>
         <v>32.150000000000006</v>
       </c>
-      <c r="N79" s="3">
+      <c r="O79" s="3">
         <v>51.67</v>
       </c>
-      <c r="Q79" s="3">
+      <c r="R79" s="3">
         <v>8.67</v>
       </c>
-      <c r="R79" s="3">
+      <c r="S79" s="3">
         <v>13</v>
       </c>
-      <c r="S79" s="3">
+      <c r="T79" s="3">
         <v>117.1</v>
       </c>
-      <c r="T79" s="3">
+      <c r="U79" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>76</v>
       </c>
@@ -3752,23 +3816,23 @@
         <f t="shared" si="2"/>
         <v>24.83</v>
       </c>
-      <c r="N80" s="3">
+      <c r="O80" s="3">
         <v>54</v>
       </c>
-      <c r="Q80" s="3">
+      <c r="R80" s="3">
         <v>5.67</v>
       </c>
-      <c r="R80" s="3">
+      <c r="S80" s="3">
         <v>16</v>
       </c>
-      <c r="S80" s="3">
+      <c r="T80" s="3">
         <v>119</v>
       </c>
-      <c r="T80" s="3">
+      <c r="U80" s="3">
         <v>42.12</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>77</v>
       </c>
@@ -3796,23 +3860,23 @@
         <f t="shared" si="2"/>
         <v>19.709999999999997</v>
       </c>
-      <c r="N81" s="3">
+      <c r="O81" s="3">
         <v>53.67</v>
       </c>
-      <c r="Q81" s="3">
+      <c r="R81" s="3">
         <v>6</v>
       </c>
-      <c r="R81" s="3">
+      <c r="S81" s="3">
         <v>9</v>
       </c>
-      <c r="S81" s="3">
+      <c r="T81" s="3">
         <v>114.92</v>
       </c>
-      <c r="T81" s="3">
+      <c r="U81" s="3">
         <v>38.44</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>78</v>
       </c>
@@ -3840,23 +3904,23 @@
         <f t="shared" si="2"/>
         <v>21.690000000000005</v>
       </c>
-      <c r="N82" s="3">
+      <c r="O82" s="3">
         <v>50.67</v>
       </c>
-      <c r="Q82" s="3">
+      <c r="R82" s="3">
         <v>9</v>
       </c>
-      <c r="R82" s="3">
+      <c r="S82" s="3">
         <v>12.67</v>
       </c>
-      <c r="S82" s="3">
+      <c r="T82" s="3">
         <v>117.8</v>
       </c>
-      <c r="T82" s="3">
+      <c r="U82" s="3">
         <v>43.09</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>79</v>
       </c>
@@ -3884,20 +3948,530 @@
         <f t="shared" si="2"/>
         <v>23.310000000000002</v>
       </c>
-      <c r="N83" s="3">
+      <c r="O83" s="3">
         <v>54.67</v>
       </c>
-      <c r="Q83" s="3">
+      <c r="R83" s="3">
         <v>6</v>
       </c>
-      <c r="R83" s="3">
+      <c r="S83" s="3">
         <v>18.329999999999998</v>
       </c>
-      <c r="S83" s="3">
+      <c r="T83" s="3">
         <v>118.27</v>
       </c>
-      <c r="T83" s="3">
+      <c r="U83" s="3">
         <v>41.16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B84" t="s">
+        <v>10</v>
+      </c>
+      <c r="D84">
+        <f>5*5.8/13.3*100</f>
+        <v>218.04511278195488</v>
+      </c>
+      <c r="E84">
+        <f>D84*V84</f>
+        <v>43.172932330827066</v>
+      </c>
+      <c r="F84">
+        <f>D84-E84</f>
+        <v>174.8721804511278</v>
+      </c>
+      <c r="G84">
+        <f>H84*E84*10</f>
+        <v>6.2169022556390976</v>
+      </c>
+      <c r="H84">
+        <v>1.44E-2</v>
+      </c>
+      <c r="V84">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="W84">
+        <v>2.7400000000000001E-2</v>
+      </c>
+      <c r="X84">
+        <f>E84/W84</f>
+        <v>1575.654464628725</v>
+      </c>
+    </row>
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B85" t="s">
+        <v>10</v>
+      </c>
+      <c r="D85">
+        <f>5*9.4/13.3*100</f>
+        <v>353.38345864661653</v>
+      </c>
+      <c r="E85">
+        <f t="shared" ref="E85:E95" si="3">D85*V85</f>
+        <v>72.090225563909769</v>
+      </c>
+      <c r="F85">
+        <f t="shared" ref="F85:F95" si="4">D85-E85</f>
+        <v>281.29323308270676</v>
+      </c>
+      <c r="G85">
+        <f>H85*E85*10</f>
+        <v>15.06685714285714</v>
+      </c>
+      <c r="H85">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="V85">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="W85">
+        <v>5.8200000000000002E-2</v>
+      </c>
+      <c r="X85">
+        <f t="shared" ref="X85:X95" si="5">E85/W85</f>
+        <v>1238.6636694829856</v>
+      </c>
+    </row>
+    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B86" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86">
+        <f>5*9.5/13.3*100</f>
+        <v>357.14285714285711</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="3"/>
+        <v>83.214285714285708</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="4"/>
+        <v>273.92857142857139</v>
+      </c>
+      <c r="G86">
+        <f>H86*E86*10</f>
+        <v>18.723214285714285</v>
+      </c>
+      <c r="H86">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="V86">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="W86">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="X86">
+        <f t="shared" si="5"/>
+        <v>1139.9217221135029</v>
+      </c>
+    </row>
+    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B87" t="s">
+        <v>10</v>
+      </c>
+      <c r="D87">
+        <f>5*6.5/13.3*100</f>
+        <v>244.36090225563908</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="3"/>
+        <v>51.804511278195484</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="4"/>
+        <v>192.55639097744358</v>
+      </c>
+      <c r="G87">
+        <f>H87*E87*10</f>
+        <v>9.1175939849624061</v>
+      </c>
+      <c r="H87">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="V87">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="W87">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="X87">
+        <f t="shared" si="5"/>
+        <v>1224.6929380188058</v>
+      </c>
+    </row>
+    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B88" t="s">
+        <v>10</v>
+      </c>
+      <c r="D88">
+        <f>5*10.6/13.3*100</f>
+        <v>398.49624060150376</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="3"/>
+        <v>98.428571428571431</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="4"/>
+        <v>300.06766917293231</v>
+      </c>
+      <c r="G88">
+        <f>H88*E88*10</f>
+        <v>21.457428571428572</v>
+      </c>
+      <c r="H88">
+        <v>2.18E-2</v>
+      </c>
+      <c r="V88">
+        <v>0.247</v>
+      </c>
+      <c r="W88">
+        <v>9.8100000000000007E-2</v>
+      </c>
+      <c r="X88">
+        <f t="shared" si="5"/>
+        <v>1003.3493519732051</v>
+      </c>
+    </row>
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B89" t="s">
+        <v>10</v>
+      </c>
+      <c r="D89">
+        <f>5*10.3/13.3*100</f>
+        <v>387.21804511278191</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="3"/>
+        <v>95.642857142857125</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="4"/>
+        <v>291.5751879699248</v>
+      </c>
+      <c r="G89">
+        <f>H89*E89*10</f>
+        <v>23.049928571428566</v>
+      </c>
+      <c r="H89">
+        <v>2.41E-2</v>
+      </c>
+      <c r="V89">
+        <v>0.247</v>
+      </c>
+      <c r="W89">
+        <v>0.1123</v>
+      </c>
+      <c r="X89">
+        <f t="shared" si="5"/>
+        <v>851.67281516346509</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B90" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90">
+        <f>9*6.1/11*100</f>
+        <v>499.09090909090912</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="3"/>
+        <v>97.821818181818188</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="4"/>
+        <v>401.26909090909095</v>
+      </c>
+      <c r="G90">
+        <f>H90*E90*10</f>
+        <v>15.553669090909093</v>
+      </c>
+      <c r="H90">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="I90">
+        <f>J90+G90</f>
+        <v>56.884385454545466</v>
+      </c>
+      <c r="J90">
+        <f>K90*F90*10</f>
+        <v>41.33071636363637</v>
+      </c>
+      <c r="K90">
+        <v>1.03E-2</v>
+      </c>
+      <c r="V90">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="W90">
+        <v>8.09E-2</v>
+      </c>
+      <c r="X90">
+        <f t="shared" si="5"/>
+        <v>1209.1695696145634</v>
+      </c>
+    </row>
+    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B91" t="s">
+        <v>10</v>
+      </c>
+      <c r="D91">
+        <f>9*8.3/11*100</f>
+        <v>679.09090909090912</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="3"/>
+        <v>147.36272727272728</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="4"/>
+        <v>531.72818181818184</v>
+      </c>
+      <c r="G91">
+        <f>H91*E91*10</f>
+        <v>26.377928181818184</v>
+      </c>
+      <c r="H91">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="I91">
+        <f t="shared" ref="I91:I95" si="6">J91+G91</f>
+        <v>117.30344727272728</v>
+      </c>
+      <c r="J91">
+        <f>K91*F91*10</f>
+        <v>90.925519090909091</v>
+      </c>
+      <c r="K91">
+        <v>1.7100000000000001E-2</v>
+      </c>
+      <c r="V91">
+        <v>0.217</v>
+      </c>
+      <c r="W91">
+        <v>0.1195</v>
+      </c>
+      <c r="X91">
+        <f t="shared" si="5"/>
+        <v>1233.1608976797263</v>
+      </c>
+    </row>
+    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B92" t="s">
+        <v>10</v>
+      </c>
+      <c r="D92">
+        <f>9*10/11*100</f>
+        <v>818.18181818181813</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="3"/>
+        <v>170.18181818181816</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="4"/>
+        <v>648</v>
+      </c>
+      <c r="G92">
+        <f>H92*E92*10</f>
+        <v>31.994181818181815</v>
+      </c>
+      <c r="H92">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="6"/>
+        <v>143.45018181818182</v>
+      </c>
+      <c r="J92">
+        <f>K92*F92*10</f>
+        <v>111.456</v>
+      </c>
+      <c r="K92">
+        <v>1.72E-2</v>
+      </c>
+      <c r="V92">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="W92">
+        <v>0.1095</v>
+      </c>
+      <c r="X92">
+        <f t="shared" si="5"/>
+        <v>1554.1718555417183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B93" t="s">
+        <v>10</v>
+      </c>
+      <c r="D93">
+        <f>9*5.9/11*100</f>
+        <v>482.72727272727269</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="3"/>
+        <v>97.993636363636369</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="4"/>
+        <v>384.73363636363632</v>
+      </c>
+      <c r="G93">
+        <f>H93*E93*10</f>
+        <v>14.699045454545454</v>
+      </c>
+      <c r="H93">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="6"/>
+        <v>54.326610000000002</v>
+      </c>
+      <c r="J93">
+        <f>K93*F93*10</f>
+        <v>39.627564545454547</v>
+      </c>
+      <c r="K93">
+        <v>1.03E-2</v>
+      </c>
+      <c r="V93">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="W93">
+        <v>0.1023</v>
+      </c>
+      <c r="X93">
+        <f t="shared" si="5"/>
+        <v>957.90455878432419</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B94" t="s">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <f>9*6.7/11*100</f>
+        <v>548.18181818181824</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="3"/>
+        <v>115.66636363636364</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="4"/>
+        <v>432.51545454545459</v>
+      </c>
+      <c r="G94">
+        <f>H94*E94*10</f>
+        <v>25.677932727272726</v>
+      </c>
+      <c r="H94">
+        <v>2.2200000000000001E-2</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="6"/>
+        <v>129.91415727272727</v>
+      </c>
+      <c r="J94">
+        <f>K94*F94*10</f>
+        <v>104.23622454545455</v>
+      </c>
+      <c r="K94">
+        <v>2.41E-2</v>
+      </c>
+      <c r="V94">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="W94">
+        <v>0.15709999999999999</v>
+      </c>
+      <c r="X94">
+        <f t="shared" si="5"/>
+        <v>736.25947572478458</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B95" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95">
+        <f>9*6.6/11*100</f>
+        <v>540</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="3"/>
+        <v>88.56</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="4"/>
+        <v>451.44</v>
+      </c>
+      <c r="G95">
+        <f>H95*E95*10</f>
+        <v>21.077280000000002</v>
+      </c>
+      <c r="H95">
+        <v>2.3800000000000002E-2</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="6"/>
+        <v>191.7216</v>
+      </c>
+      <c r="J95">
+        <f>K95*F95*10</f>
+        <v>170.64431999999999</v>
+      </c>
+      <c r="K95">
+        <v>3.78E-2</v>
+      </c>
+      <c r="V95">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="W95">
+        <v>0.14630000000000001</v>
+      </c>
+      <c r="X95">
+        <f t="shared" si="5"/>
+        <v>605.33151059466843</v>
       </c>
     </row>
   </sheetData>
@@ -4409,8 +4983,8 @@
   <cols>
     <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -9332,9 +9906,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Just trying to get the test set actually graphing things
</commit_message>
<xml_diff>
--- a/Prototypes/Teff/Observed.xlsx
+++ b/Prototypes/Teff/Observed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8F43E8-4E89-4B68-B052-64333769120B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9CFD33-8937-40D4-8F7B-AD029270597D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,12 +407,6 @@
     <t>HeadingDAS</t>
   </si>
   <si>
-    <t>GrainN</t>
-  </si>
-  <si>
-    <t>BiomassN</t>
-  </si>
-  <si>
     <t>Habro2012Control</t>
   </si>
   <si>
@@ -723,6 +717,12 @@
   </si>
   <si>
     <t>Teff.Grain.Wt</t>
+  </si>
+  <si>
+    <t>Teff.AboveGround.N</t>
+  </si>
+  <si>
+    <t>Teff.Grain.N</t>
   </si>
 </sst>
 </file>
@@ -2076,7 +2076,7 @@
   <dimension ref="A1:X95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2095,34 +2095,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" t="s">
         <v>165</v>
       </c>
-      <c r="E1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" t="s">
-        <v>61</v>
-      </c>
-      <c r="H1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I1" t="s">
-        <v>62</v>
-      </c>
       <c r="J1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L1" t="s">
         <v>4</v>
@@ -2143,25 +2143,25 @@
         <v>8</v>
       </c>
       <c r="R1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S1" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" t="s">
         <v>79</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>80</v>
       </c>
-      <c r="T1" t="s">
-        <v>81</v>
-      </c>
-      <c r="U1" t="s">
-        <v>82</v>
-      </c>
       <c r="V1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="W1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="X1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -2945,7 +2945,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
@@ -2979,7 +2979,7 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
@@ -2996,7 +2996,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="49" spans="1:17">
       <c r="A49" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
@@ -3047,7 +3047,7 @@
     </row>
     <row r="50" spans="1:17">
       <c r="A50" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
@@ -3064,7 +3064,7 @@
     </row>
     <row r="51" spans="1:17">
       <c r="A51" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
@@ -3081,7 +3081,7 @@
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
@@ -3098,7 +3098,7 @@
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
@@ -3115,7 +3115,7 @@
     </row>
     <row r="54" spans="1:17">
       <c r="A54" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
@@ -3132,7 +3132,7 @@
     </row>
     <row r="55" spans="1:17">
       <c r="A55" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B55" t="s">
         <v>9</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="56" spans="1:17">
       <c r="A56" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="57" spans="1:17">
       <c r="A57" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
@@ -3183,7 +3183,7 @@
     </row>
     <row r="58" spans="1:17">
       <c r="A58" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="59" spans="1:17">
       <c r="A59" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="68" spans="1:21">
       <c r="A68" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
@@ -3419,7 +3419,7 @@
     </row>
     <row r="69" spans="1:21">
       <c r="A69" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
@@ -3463,7 +3463,7 @@
     </row>
     <row r="70" spans="1:21">
       <c r="A70" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
@@ -3507,7 +3507,7 @@
     </row>
     <row r="71" spans="1:21">
       <c r="A71" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
@@ -3551,7 +3551,7 @@
     </row>
     <row r="72" spans="1:21">
       <c r="A72" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
@@ -3595,7 +3595,7 @@
     </row>
     <row r="73" spans="1:21">
       <c r="A73" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
         <v>9</v>
@@ -3639,7 +3639,7 @@
     </row>
     <row r="74" spans="1:21">
       <c r="A74" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B74" t="s">
         <v>9</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="75" spans="1:21">
       <c r="A75" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="76" spans="1:21">
       <c r="A76" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
@@ -3771,7 +3771,7 @@
     </row>
     <row r="77" spans="1:21">
       <c r="A77" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
@@ -3815,7 +3815,7 @@
     </row>
     <row r="78" spans="1:21">
       <c r="A78" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B78" t="s">
         <v>9</v>
@@ -3859,7 +3859,7 @@
     </row>
     <row r="79" spans="1:21">
       <c r="A79" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
@@ -3903,7 +3903,7 @@
     </row>
     <row r="80" spans="1:21">
       <c r="A80" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
@@ -3947,7 +3947,7 @@
     </row>
     <row r="81" spans="1:24">
       <c r="A81" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
@@ -3991,7 +3991,7 @@
     </row>
     <row r="82" spans="1:24">
       <c r="A82" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
@@ -4035,7 +4035,7 @@
     </row>
     <row r="83" spans="1:24">
       <c r="A83" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="84" spans="1:24">
       <c r="A84" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
@@ -4116,7 +4116,7 @@
     </row>
     <row r="85" spans="1:24">
       <c r="A85" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -4153,7 +4153,7 @@
     </row>
     <row r="86" spans="1:24">
       <c r="A86" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="87" spans="1:24">
       <c r="A87" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="88" spans="1:24">
       <c r="A88" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
@@ -4264,7 +4264,7 @@
     </row>
     <row r="89" spans="1:24">
       <c r="A89" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
@@ -4301,7 +4301,7 @@
     </row>
     <row r="90" spans="1:24">
       <c r="A90" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
@@ -4349,7 +4349,7 @@
     </row>
     <row r="91" spans="1:24">
       <c r="A91" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
@@ -4397,7 +4397,7 @@
     </row>
     <row r="92" spans="1:24">
       <c r="A92" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
@@ -4445,7 +4445,7 @@
     </row>
     <row r="93" spans="1:24">
       <c r="A93" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
@@ -4493,7 +4493,7 @@
     </row>
     <row r="94" spans="1:24">
       <c r="A94" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
@@ -4541,7 +4541,7 @@
     </row>
     <row r="95" spans="1:24">
       <c r="A95" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
@@ -4618,33 +4618,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
         <v>134</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>135</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>137</v>
       </c>
-      <c r="H1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" t="s">
-        <v>139</v>
-      </c>
       <c r="J1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="1">
         <f>DATE(2012,3,11)+C2</f>
@@ -4677,7 +4677,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B14" si="0">DATE(2012,3,11)+C3</f>
@@ -4710,7 +4710,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
@@ -4743,7 +4743,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
@@ -4776,7 +4776,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
@@ -4809,7 +4809,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
@@ -4842,7 +4842,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
@@ -4875,7 +4875,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
@@ -4908,7 +4908,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
@@ -4941,7 +4941,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
@@ -4974,7 +4974,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
@@ -5007,7 +5007,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
@@ -5040,7 +5040,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
@@ -5285,13 +5285,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
         <v>145</v>
-      </c>
-      <c r="C1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5912,13 +5912,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -5927,10 +5927,10 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -6786,13 +6786,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -7177,13 +7177,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="19.2" customHeight="1">
@@ -9414,13 +9414,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -9429,13 +9429,13 @@
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1">
@@ -10026,24 +10026,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
         <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B2">
         <v>9</v>
@@ -10063,7 +10063,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3">
         <v>10.5</v>
@@ -10080,7 +10080,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4">
         <v>12</v>
@@ -10097,7 +10097,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B5">
         <v>13.5</v>
@@ -10117,7 +10117,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -10137,7 +10137,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B7">
         <v>16.5</v>
@@ -10157,7 +10157,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B8">
         <v>9</v>
@@ -10177,7 +10177,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B9">
         <v>10.5</v>
@@ -10194,7 +10194,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B10">
         <v>12</v>
@@ -10211,7 +10211,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B11">
         <v>13.5</v>
@@ -10231,7 +10231,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B12">
         <v>15</v>
@@ -10251,7 +10251,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B13">
         <v>16.5</v>
@@ -10268,7 +10268,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -10288,7 +10288,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B15">
         <v>10.5</v>
@@ -10305,7 +10305,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B16">
         <v>12</v>
@@ -10322,7 +10322,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B17">
         <v>13.5</v>
@@ -10342,7 +10342,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B18">
         <v>15</v>
@@ -10362,7 +10362,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B19">
         <v>16.5</v>
@@ -10382,7 +10382,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B20">
         <v>9</v>
@@ -10402,7 +10402,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B21">
         <v>10.5</v>
@@ -10419,7 +10419,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B22">
         <v>12</v>
@@ -10436,7 +10436,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B23">
         <v>13.5</v>
@@ -10456,7 +10456,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B24">
         <v>15</v>
@@ -10476,7 +10476,7 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B25">
         <v>16.5</v>
@@ -10521,33 +10521,33 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
         <v>134</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>135</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>137</v>
       </c>
-      <c r="H1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" t="s">
-        <v>139</v>
-      </c>
       <c r="J1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1">
         <f>DATE(2011,3,7)+C2</f>
@@ -10580,7 +10580,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" s="1">
         <f t="shared" ref="B3:B17" si="0">DATE(2011,3,7)+C3</f>
@@ -10613,7 +10613,7 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" si="0"/>
@@ -10646,7 +10646,7 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B5" s="1">
         <f t="shared" si="0"/>
@@ -10679,7 +10679,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
@@ -10712,7 +10712,7 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
@@ -10745,7 +10745,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
@@ -10778,7 +10778,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
@@ -10811,7 +10811,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
@@ -10844,7 +10844,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
@@ -10877,7 +10877,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
@@ -10910,7 +10910,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
@@ -10943,7 +10943,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
@@ -10976,7 +10976,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
@@ -11009,7 +11009,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
@@ -11042,7 +11042,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
convert to nutrient and start fixing stem model
</commit_message>
<xml_diff>
--- a/Prototypes/Teff/Observed.xlsx
+++ b/Prototypes/Teff/Observed.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4235ABC-5450-4BAE-8DED-230376F029CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5AA2E5-49FD-4429-B42A-FA387C1B70C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedHarvestData" sheetId="1" r:id="rId1"/>
@@ -2075,8 +2075,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2:V11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="7635" ySplit="585" topLeftCell="I66" activePane="bottomLeft"/>
+      <selection sqref="A1:XFD1"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84:C89"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4126,6 +4130,9 @@
       <c r="B84" t="s">
         <v>9</v>
       </c>
+      <c r="C84" s="4">
+        <v>38261</v>
+      </c>
       <c r="D84">
         <f>5*5.8/13.3*100</f>
         <v>218.04511278195488</v>
@@ -4163,6 +4170,9 @@
       <c r="B85" t="s">
         <v>9</v>
       </c>
+      <c r="C85" s="4">
+        <v>38261</v>
+      </c>
       <c r="D85">
         <f>5*9.4/13.3*100</f>
         <v>353.38345864661653</v>
@@ -4200,6 +4210,9 @@
       <c r="B86" t="s">
         <v>9</v>
       </c>
+      <c r="C86" s="4">
+        <v>38261</v>
+      </c>
       <c r="D86">
         <f>5*9.5/13.3*100</f>
         <v>357.14285714285711</v>
@@ -4237,6 +4250,9 @@
       <c r="B87" t="s">
         <v>9</v>
       </c>
+      <c r="C87" s="4">
+        <v>38261</v>
+      </c>
       <c r="D87">
         <f>5*6.5/13.3*100</f>
         <v>244.36090225563908</v>
@@ -4274,6 +4290,9 @@
       <c r="B88" t="s">
         <v>9</v>
       </c>
+      <c r="C88" s="4">
+        <v>38261</v>
+      </c>
       <c r="D88">
         <f>5*10.6/13.3*100</f>
         <v>398.49624060150376</v>
@@ -4310,6 +4329,9 @@
       </c>
       <c r="B89" t="s">
         <v>9</v>
+      </c>
+      <c r="C89" s="4">
+        <v>38261</v>
       </c>
       <c r="D89">
         <f>5*10.3/13.3*100</f>

</xml_diff>